<commit_message>
eda rerun, now need to update company names/mentions
</commit_message>
<xml_diff>
--- a/Output/All Data EDA/Tabular EDA/Numeric_Summary_Statistics.xlsx
+++ b/Output/All Data EDA/Tabular EDA/Numeric_Summary_Statistics.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G113"/>
+  <dimension ref="A1:G159"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,1265 +473,1265 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Altman's Z Score</t>
+          <t>Difference in Cash Per Share from prior fixed quarter</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1.88039655703126</v>
+        <v>-0.005885481493750157</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.908811003922197</v>
+        <v>-69.19201533743652</v>
       </c>
       <c r="D2" t="n">
-        <v>1.609280414349376</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>7.557017289289491</v>
+        <v>69.01598984285708</v>
       </c>
       <c r="F2" t="n">
-        <v>1.281657788470586</v>
+        <v>4.540626760945713</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Altman's Z Score</t>
+          <t>Additional Change Ratios</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Accounts Payable (Balance Sheet)</t>
+          <t>Difference in Cash Ratio from prior fixed quarter</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>966256179.2351079</v>
+        <v>0.05472192724269662</v>
       </c>
       <c r="C3" t="n">
-        <v>-237651171</v>
+        <v>-53.11199223231032</v>
       </c>
       <c r="D3" t="n">
-        <v>358675500</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>11433000000</v>
+        <v>53.11264011409434</v>
       </c>
       <c r="F3" t="n">
-        <v>1564143869.543608</v>
+        <v>3.975183628377203</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Financial Statements</t>
+          <t>Additional Change Ratios</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Accounts Payable (Cash Flow Statement)</t>
+          <t>Difference in Debt Ratio (Alternative) from prior fixed quarter</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>5115097.343065695</v>
+        <v>0.002793981004582174</v>
       </c>
       <c r="C4" t="n">
-        <v>-321769000</v>
+        <v>-0.7593652759723031</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>1789652000</v>
+        <v>0.7798541497671294</v>
       </c>
       <c r="F4" t="n">
-        <v>82020828.63734347</v>
+        <v>0.0497062907633386</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Financial Statements</t>
+          <t>Additional Change Ratios</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Accounts Receivables</t>
+          <t>Difference in Debt Ratio from prior fixed quarter</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-11276972.00588986</v>
+        <v>0.003452306388638653</v>
       </c>
       <c r="C5" t="n">
-        <v>-544000000</v>
+        <v>-0.822900692982916</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>325000000</v>
+        <v>0.8275259746158774</v>
       </c>
       <c r="F5" t="n">
-        <v>91302900.98173185</v>
+        <v>0.04998083056218851</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Financial Statements</t>
+          <t>Additional Change Ratios</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Accumulated Other Comprehensive Income (Loss)</t>
+          <t>Difference in Debt to Equity Ratio from prior fixed quarter</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-404904065.7678509</v>
+        <v>-1.898410068169009</v>
       </c>
       <c r="C6" t="n">
-        <v>-5290000000</v>
+        <v>-1915.807284900496</v>
       </c>
       <c r="D6" t="n">
-        <v>-74923500</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>431595000</v>
+        <v>1892.365911273534</v>
       </c>
       <c r="F6" t="n">
-        <v>880562727.6246001</v>
+        <v>113.7101510000325</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Financial Statements</t>
+          <t>Additional Change Ratios</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Capital Expenditure</t>
+          <t>Difference in EBIT to Revenue from prior fixed quarter</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-192838993.5675663</v>
+        <v>-0.001161761673700804</v>
       </c>
       <c r="C7" t="n">
-        <v>-1867000000</v>
+        <v>-0.6644020785350223</v>
       </c>
       <c r="D7" t="n">
-        <v>-61000000</v>
+        <v>0.001081603567715403</v>
       </c>
       <c r="E7" t="n">
-        <v>412700</v>
+        <v>0.5899817517267851</v>
       </c>
       <c r="F7" t="n">
-        <v>309755067.3626994</v>
+        <v>0.08825665642255129</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Financial Statements</t>
+          <t>Additional Change Ratios</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Capital Lease Obligations</t>
+          <t>Difference in Enterprise Value Multiplier from prior fixed quarter</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>25062333.47838736</v>
+        <v>0.2491568451726167</v>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>-1036.949704550451</v>
       </c>
       <c r="D8" t="n">
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>9056234000</v>
+        <v>1036.949704550451</v>
       </c>
       <c r="F8" t="n">
-        <v>228139330.3327314</v>
+        <v>121.2173001727553</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Financial Statements</t>
+          <t>Additional Change Ratios</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Cash and Cash Equivalents</t>
+          <t>Difference in Equity Multiplier from prior fixed quarter</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>869139501.4696107</v>
+        <v>-1.328889637483984</v>
       </c>
       <c r="C9" t="n">
+        <v>-1292.745478544182</v>
+      </c>
+      <c r="D9" t="n">
         <v>0</v>
       </c>
-      <c r="D9" t="n">
-        <v>334747500</v>
-      </c>
       <c r="E9" t="n">
-        <v>9223000000</v>
+        <v>1292.745478544182</v>
       </c>
       <c r="F9" t="n">
-        <v>1373785187.87019</v>
+        <v>80.06044276699807</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Financial Statements</t>
+          <t>Additional Change Ratios</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Cash and Short Term Investments</t>
+          <t>Difference in Free Cash Flow Per Share from prior fixed quarter</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1064264890.379766</v>
+        <v>0.01274558462660912</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>-10.67973555619431</v>
       </c>
       <c r="D10" t="n">
-        <v>365150000</v>
+        <v>0.0138105172134424</v>
       </c>
       <c r="E10" t="n">
-        <v>15601000000</v>
+        <v>10.67973555619431</v>
       </c>
       <c r="F10" t="n">
-        <v>1892893943.18019</v>
+        <v>1.825740477357688</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Financial Statements</t>
+          <t>Additional Change Ratios</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Cash at Beginning of Period</t>
+          <t>Difference in Free Cash Flow to Operating Cash Flow from prior fixed quarter</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>875066189.857394</v>
+        <v>0.00722504326973661</v>
       </c>
       <c r="C11" t="n">
-        <v>-2556000</v>
+        <v>-13.3973183486574</v>
       </c>
       <c r="D11" t="n">
-        <v>336188500</v>
+        <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>9610000000</v>
+        <v>13.3973183486574</v>
       </c>
       <c r="F11" t="n">
-        <v>1399673823.880652</v>
+        <v>2.399213392400922</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Financial Statements</t>
+          <t>Additional Change Ratios</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Cash at End of Period</t>
+          <t>Difference in Operating Cash Flow Per Share from prior fixed quarter</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>881467356.7073531</v>
+        <v>0.0130409495527535</v>
       </c>
       <c r="C12" t="n">
-        <v>-154400</v>
+        <v>-12.80132177308388</v>
       </c>
       <c r="D12" t="n">
-        <v>337800000</v>
+        <v>0.01650804498077652</v>
       </c>
       <c r="E12" t="n">
-        <v>9743000000</v>
+        <v>12.80132177308388</v>
       </c>
       <c r="F12" t="n">
-        <v>1410805303.471063</v>
+        <v>1.792410649362168</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Financial Statements</t>
+          <t>Additional Change Ratios</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Change in Working Capital</t>
+          <t>Difference in Operating Cash Flow to Sales from prior fixed quarter</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-17622464.71814562</v>
+        <v>0.0003413407855667715</v>
       </c>
       <c r="C13" t="n">
-        <v>-870000000</v>
+        <v>-0.7880429390181567</v>
       </c>
       <c r="D13" t="n">
-        <v>-2509500</v>
+        <v>0.005058667191473354</v>
       </c>
       <c r="E13" t="n">
-        <v>756000000</v>
+        <v>0.7880429390181567</v>
       </c>
       <c r="F13" t="n">
-        <v>183386926.9245657</v>
+        <v>0.1426467876582321</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Financial Statements</t>
+          <t>Additional Change Ratios</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Common Stock</t>
+          <t>Difference in Quick Ratio from prior fixed quarter</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>333701836.2958734</v>
+        <v>-0.00448297755694608</v>
       </c>
       <c r="C14" t="n">
-        <v>-539800</v>
+        <v>-5.298313981388063</v>
       </c>
       <c r="D14" t="n">
-        <v>3962000</v>
+        <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>9817134000</v>
+        <v>5.157504796379142</v>
       </c>
       <c r="F14" t="n">
-        <v>936073406.5785795</v>
+        <v>0.5139364647545841</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Financial Statements</t>
+          <t>Additional Change Ratios</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Common Stock Issued</t>
+          <t>Difference in Return on Assets from prior fixed quarter</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>44261851.93875144</v>
+        <v>-0.000168938716748184</v>
       </c>
       <c r="C15" t="n">
-        <v>-3572000</v>
+        <v>-0.09752050308939972</v>
       </c>
       <c r="D15" t="n">
-        <v>43000</v>
+        <v>2.542687905807486e-05</v>
       </c>
       <c r="E15" t="n">
-        <v>1111490728</v>
+        <v>0.09752050308939972</v>
       </c>
       <c r="F15" t="n">
-        <v>123285381.7682303</v>
+        <v>0.01467658135252018</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Financial Statements</t>
+          <t>Additional Change Ratios</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Common Stock Repurchased</t>
+          <t>Difference in Return on Capital Employed from prior fixed quarter</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-78688233.14151685</v>
+        <v>-0.0003542161313017087</v>
       </c>
       <c r="C16" t="n">
-        <v>-2086545366</v>
+        <v>-0.1389387122217676</v>
       </c>
       <c r="D16" t="n">
-        <v>-797000</v>
+        <v>2.222988698973721e-05</v>
       </c>
       <c r="E16" t="n">
-        <v>545656614.524539</v>
+        <v>0.1340228638339568</v>
       </c>
       <c r="F16" t="n">
-        <v>187838839.6578202</v>
+        <v>0.01982837702502859</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Financial Statements</t>
+          <t>Additional Change Ratios</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Cost and Expenses</t>
+          <t>Difference in Return on Equity from prior fixed quarter</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>2339756005.828557</v>
+        <v>-0.001552393369845179</v>
       </c>
       <c r="C17" t="n">
-        <v>-2495000</v>
+        <v>-2.106410433134444</v>
       </c>
       <c r="D17" t="n">
-        <v>1130100000</v>
+        <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>22769000000</v>
+        <v>2.106410433134444</v>
       </c>
       <c r="F17" t="n">
-        <v>3398867286.325137</v>
+        <v>0.2259711758418302</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Financial Statements</t>
+          <t>Additional Change Ratios</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Cost of Revenue</t>
+          <t>Differnce in Current Ratio from prior fixed quarter</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>1639068160.073856</v>
+        <v>-0.0001572768989736388</v>
       </c>
       <c r="C18" t="n">
-        <v>-3094000</v>
+        <v>-6.869039999447338</v>
       </c>
       <c r="D18" t="n">
-        <v>791749000</v>
+        <v>0</v>
       </c>
       <c r="E18" t="n">
-        <v>18303000000</v>
+        <v>6.967837335846087</v>
       </c>
       <c r="F18" t="n">
-        <v>2432969396.593343</v>
+        <v>0.6067301798395416</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Financial Statements</t>
+          <t>Additional Change Ratios</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Debt Repayment</t>
+          <t>Cash Per Share</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>-246924032.2008753</v>
+        <v>4.568656495954678</v>
       </c>
       <c r="C19" t="n">
-        <v>-3001000000</v>
+        <v>0.001766180435406438</v>
       </c>
       <c r="D19" t="n">
-        <v>-32044500</v>
+        <v>2.131618652155985</v>
       </c>
       <c r="E19" t="n">
-        <v>200</v>
+        <v>69.90892149760721</v>
       </c>
       <c r="F19" t="n">
-        <v>471308141.5025936</v>
+        <v>9.643451982425368</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Financial Statements</t>
+          <t>Additional Ratios</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Deferred Income Tax</t>
+          <t>Cash Ratio</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>6021092.61919504</v>
+        <v>1.206559919398094</v>
       </c>
       <c r="C20" t="n">
-        <v>-253000000</v>
+        <v>0.00088524890948865</v>
       </c>
       <c r="D20" t="n">
-        <v>64500</v>
+        <v>0.2831355750333205</v>
       </c>
       <c r="E20" t="n">
-        <v>1850454000</v>
+        <v>53.16729078452483</v>
       </c>
       <c r="F20" t="n">
-        <v>59026597.61897585</v>
+        <v>6.229328037676222</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Financial Statements</t>
+          <t>Additional Ratios</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Deferred Revenue</t>
+          <t>Current Ratio</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>309581598.2351098</v>
+        <v>1.93304321581549</v>
       </c>
       <c r="C21" t="n">
-        <v>-116912000</v>
+        <v>0.3481486170618474</v>
       </c>
       <c r="D21" t="n">
-        <v>48000000</v>
+        <v>1.579189855674458</v>
       </c>
       <c r="E21" t="n">
-        <v>4918100000</v>
+        <v>7.928402465484342</v>
       </c>
       <c r="F21" t="n">
-        <v>646673378.8820082</v>
+        <v>1.333643455007153</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Financial Statements</t>
+          <t>Additional Ratios</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Depreciation and Amortization (Cash Flow Statement)</t>
+          <t>Debt Ratio</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>142785944.038052</v>
+        <v>0.350987874245856</v>
       </c>
       <c r="C22" t="n">
-        <v>-675312</v>
+        <v>0.0004561513713548658</v>
       </c>
       <c r="D22" t="n">
-        <v>53814500</v>
+        <v>0.324847882776605</v>
       </c>
       <c r="E22" t="n">
-        <v>1529000000</v>
+        <v>0.9377814085115745</v>
       </c>
       <c r="F22" t="n">
-        <v>212219854.1436878</v>
+        <v>0.1853799506653347</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Financial Statements</t>
+          <t>Additional Ratios</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Depreciation and Amortization (Income Statement)</t>
+          <t>Debt Ratio (Alternative Definition)</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>141427421.895724</v>
+        <v>0.6523912817946774</v>
       </c>
       <c r="C23" t="n">
-        <v>-1550000</v>
+        <v>0.2822043164122687</v>
       </c>
       <c r="D23" t="n">
-        <v>54944500</v>
+        <v>0.6399998029869639</v>
       </c>
       <c r="E23" t="n">
-        <v>1371000000</v>
+        <v>1.215863568260637</v>
       </c>
       <c r="F23" t="n">
-        <v>204346754.1524246</v>
+        <v>0.1748678568279178</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Financial Statements</t>
+          <t>Additional Ratios</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Diluted EPS</t>
+          <t>Debt to Equity Ratio</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.5150406172839506</v>
+        <v>-34.63369110509741</v>
       </c>
       <c r="C24" t="n">
-        <v>-156.36</v>
+        <v>-1890.408491259598</v>
       </c>
       <c r="D24" t="n">
-        <v>0.51</v>
+        <v>1.697819314641745</v>
       </c>
       <c r="E24" t="n">
-        <v>49.73</v>
+        <v>25.39879364089801</v>
       </c>
       <c r="F24" t="n">
-        <v>3.268257389612775</v>
+        <v>256.0235338216692</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Financial Statements</t>
+          <t>Additional Ratios</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Dividends Paid</t>
+          <t>EBIT to Revenue</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>-91477627.47726284</v>
+        <v>0.1226322353436107</v>
       </c>
       <c r="C25" t="n">
-        <v>-1233000000</v>
+        <v>-0.2553314646720286</v>
       </c>
       <c r="D25" t="n">
-        <v>-21000500</v>
+        <v>0.1127990755845568</v>
       </c>
       <c r="E25" t="n">
-        <v>0</v>
+        <v>0.4697487077376978</v>
       </c>
       <c r="F25" t="n">
-        <v>182607289.0574467</v>
+        <v>0.1221050783762077</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Financial Statements</t>
+          <t>Additional Ratios</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>EBITDA</t>
+          <t>Enterprise Value Multiplier</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>446138301.6032988</v>
+        <v>59.08193440956648</v>
       </c>
       <c r="C26" t="n">
-        <v>-66200000</v>
+        <v>-309.7499803541392</v>
       </c>
       <c r="D26" t="n">
-        <v>194050000</v>
+        <v>40.66931880108991</v>
       </c>
       <c r="E26" t="n">
-        <v>4410000000</v>
+        <v>727.199724196312</v>
       </c>
       <c r="F26" t="n">
-        <v>643419252.0193411</v>
+        <v>125.9286471388882</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Financial Statements</t>
+          <t>Additional Ratios</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>EBITDA Ratio</t>
+          <t>Equity Multiplier</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.2007015508214462</v>
+        <v>-22.79306581040573</v>
       </c>
       <c r="C27" t="n">
-        <v>-5.769041769</v>
+        <v>-1270.102609475951</v>
       </c>
       <c r="D27" t="n">
-        <v>0.1723145856</v>
+        <v>2.70539627680465</v>
       </c>
       <c r="E27" t="n">
-        <v>2.1555001457</v>
+        <v>22.64286906823081</v>
       </c>
       <c r="F27" t="n">
-        <v>0.2168446357479668</v>
+        <v>175.0803655170625</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Financial Statements</t>
+          <t>Additional Ratios</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>EPS</t>
+          <t>Free Cash Flow Per Share</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.5280683421516755</v>
+        <v>0.5689020212686842</v>
       </c>
       <c r="C28" t="n">
-        <v>-156.36</v>
+        <v>-2.975510204081633</v>
       </c>
       <c r="D28" t="n">
-        <v>0.52</v>
+        <v>0.3941176470588235</v>
       </c>
       <c r="E28" t="n">
-        <v>53.75</v>
+        <v>7.704225352112676</v>
       </c>
       <c r="F28" t="n">
-        <v>3.293867924205674</v>
+        <v>1.516815998315839</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Financial Statements</t>
+          <t>Additional Ratios</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Effect of Foreign Exchange Changes on Cash</t>
+          <t>Free Cash Flow to Operating Cash Flow</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>-1653388.245807762</v>
+        <v>0.7174172058440923</v>
       </c>
       <c r="C29" t="n">
-        <v>-65000000</v>
+        <v>-2.416785561772159</v>
       </c>
       <c r="D29" t="n">
-        <v>0</v>
+        <v>0.6577780405605156</v>
       </c>
       <c r="E29" t="n">
-        <v>52000000</v>
+        <v>10.98053278688525</v>
       </c>
       <c r="F29" t="n">
-        <v>11180607.84801697</v>
+        <v>1.856563426698278</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Financial Statements</t>
+          <t>Additional Ratios</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Free Cash Flow</t>
+          <t>Operating Cash Flow Per Share</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>157084973.5468172</v>
+        <v>1.475889389862626</v>
       </c>
       <c r="C30" t="n">
-        <v>-541000000</v>
+        <v>-0.983249581239531</v>
       </c>
       <c r="D30" t="n">
-        <v>51192500</v>
+        <v>1.044190970532091</v>
       </c>
       <c r="E30" t="n">
-        <v>2683000000</v>
+        <v>11.81807219184435</v>
       </c>
       <c r="F30" t="n">
-        <v>388980015.5277251</v>
+        <v>1.916163549171745</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Financial Statements</t>
+          <t>Additional Ratios</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>General and Administrative Expenses</t>
+          <t>Operating Cash Flow to Sales</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>153358448.1222456</v>
+        <v>0.1644547996979013</v>
       </c>
       <c r="C31" t="n">
-        <v>-2738500</v>
+        <v>-0.1483462352224627</v>
       </c>
       <c r="D31" t="n">
-        <v>32647000</v>
+        <v>0.1417813033437092</v>
       </c>
       <c r="E31" t="n">
-        <v>2007000000</v>
+        <v>0.639696703795694</v>
       </c>
       <c r="F31" t="n">
-        <v>301738888.2690312</v>
+        <v>0.1520418647827099</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Financial Statements</t>
+          <t>Additional Ratios</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Goodwill</t>
+          <t>Quick Ratio</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>2002690830.527137</v>
+        <v>1.364828247394939</v>
       </c>
       <c r="C32" t="n">
-        <v>-202702100</v>
+        <v>0.000609344706488944</v>
       </c>
       <c r="D32" t="n">
-        <v>630531000</v>
+        <v>1.1506052141527</v>
       </c>
       <c r="E32" t="n">
-        <v>23389000000</v>
+        <v>6.118069926017397</v>
       </c>
       <c r="F32" t="n">
-        <v>3533369156.815275</v>
+        <v>0.9763887067772591</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Financial Statements</t>
+          <t>Additional Ratios</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Goodwill and Intangible Assets</t>
+          <t>Return on Assets</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>3124212237.48229</v>
+        <v>0.01257075055979723</v>
       </c>
       <c r="C33" t="n">
-        <v>-1618944000</v>
+        <v>-0.03481041526367147</v>
       </c>
       <c r="D33" t="n">
-        <v>966716000</v>
+        <v>0.01101083200318583</v>
       </c>
       <c r="E33" t="n">
-        <v>37123000000</v>
+        <v>0.06271008782572825</v>
       </c>
       <c r="F33" t="n">
-        <v>5678672562.168402</v>
+        <v>0.01535977907747937</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Financial Statements</t>
+          <t>Additional Ratios</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Gross Profit</t>
+          <t>Return on Capital Employed</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>868732901.3275729</v>
+        <v>0.02803132080879312</v>
       </c>
       <c r="C34" t="n">
-        <v>-7195000</v>
+        <v>-0.02549643371085762</v>
       </c>
       <c r="D34" t="n">
-        <v>379801000</v>
+        <v>0.02393410852713178</v>
       </c>
       <c r="E34" t="n">
-        <v>9223000000</v>
+        <v>0.11344227851091</v>
       </c>
       <c r="F34" t="n">
-        <v>1372085330.979887</v>
+        <v>0.02595739360811902</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Financial Statements</t>
+          <t>Additional Ratios</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Gross Profit Ratio</t>
+          <t>Return on Equity</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.3670792599708113</v>
+        <v>0.01243144335268753</v>
       </c>
       <c r="C35" t="n">
-        <v>-5.6527436527</v>
+        <v>-1.32349570187112</v>
       </c>
       <c r="D35" t="n">
-        <v>0.34244958575</v>
+        <v>0.03036560184622859</v>
       </c>
       <c r="E35" t="n">
-        <v>2.3163345465</v>
+        <v>0.7829147312633248</v>
       </c>
       <c r="F35" t="n">
-        <v>0.2611523972841556</v>
+        <v>0.2513884881911687</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Financial Statements</t>
+          <t>Additional Ratios</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Income Before Tax</t>
+          <t>Altman's Z Score</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>256118983.2542</v>
+        <v>1.877594340469448</v>
       </c>
       <c r="C36" t="n">
-        <v>-353153000</v>
+        <v>-0.908811003922197</v>
       </c>
       <c r="D36" t="n">
-        <v>92535500</v>
+        <v>1.609265181015041</v>
       </c>
       <c r="E36" t="n">
-        <v>2951000000</v>
+        <v>7.557017289289491</v>
       </c>
       <c r="F36" t="n">
-        <v>434784626.4338911</v>
+        <v>1.2786221473992</v>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>Financial Statements</t>
+          <t>Altman's Z Score</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Income Before Tax Ratio</t>
+          <t>Difference in Altman's Z from prior fixed quarter</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>0.07147083996908288</v>
+        <v>-0.006540267071068333</v>
       </c>
       <c r="C37" t="n">
-        <v>-9.3813885267</v>
+        <v>-4.838973791152402</v>
       </c>
       <c r="D37" t="n">
-        <v>0.09255891704999999</v>
+        <v>0.01163468270635104</v>
       </c>
       <c r="E37" t="n">
-        <v>2.678365705</v>
+        <v>4.413579727743642</v>
       </c>
       <c r="F37" t="n">
-        <v>0.3464772867408581</v>
+        <v>0.3856868302571551</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Financial Statements</t>
+          <t>Change Ratios</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Income Tax Expense</t>
+          <t>Difference in EBITDA Ratio from prior fixed quarter</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>69610448.40986587</v>
+        <v>-0.0001407655290796876</v>
       </c>
       <c r="C38" t="n">
-        <v>-119131000</v>
+        <v>-3.0949917076</v>
       </c>
       <c r="D38" t="n">
-        <v>22400000</v>
+        <v>0.0019359146</v>
       </c>
       <c r="E38" t="n">
-        <v>736000000</v>
+        <v>5.2011172407</v>
       </c>
       <c r="F38" t="n">
-        <v>121357794.2573632</v>
+        <v>0.1642255661511772</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Financial Statements</t>
+          <t>Change Ratios</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Intangible Assets</t>
+          <t>Difference in Gross Profit Ratio from prior fixed quarter</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>838566674.6369867</v>
+        <v>-0.000416786049573425</v>
       </c>
       <c r="C39" t="n">
-        <v>-421000</v>
+        <v>-3.1565329815</v>
       </c>
       <c r="D39" t="n">
-        <v>169050000</v>
+        <v>0.0009633779000000064</v>
       </c>
       <c r="E39" t="n">
-        <v>14110100000</v>
+        <v>5.2263285584</v>
       </c>
       <c r="F39" t="n">
-        <v>1786919275.207674</v>
+        <v>0.1527159141260995</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Financial Statements</t>
+          <t>Change Ratios</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Interest Expense</t>
+          <t>Difference in Income Before Tax Ratio from prior fixed quarter</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>46670431.96120407</v>
+        <v>-0.00289669296420403</v>
       </c>
       <c r="C40" t="n">
-        <v>-16400000</v>
+        <v>-6.694328303200001</v>
       </c>
       <c r="D40" t="n">
-        <v>23050000</v>
+        <v>0.001660488200000004</v>
       </c>
       <c r="E40" t="n">
-        <v>386000000</v>
+        <v>6.432117967</v>
       </c>
       <c r="F40" t="n">
-        <v>61968392.6251269</v>
+        <v>0.3304192731985123</v>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>Financial Statements</t>
+          <t>Change Ratios</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Interest Income</t>
+          <t>Difference in Net Income Ratio from prior fixed quarter</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>2377179.839086681</v>
+        <v>-0.002977571413777454</v>
       </c>
       <c r="C41" t="n">
-        <v>-62900</v>
+        <v>-7.134891722999999</v>
       </c>
       <c r="D41" t="n">
-        <v>0</v>
+        <v>0.001254916500000008</v>
       </c>
       <c r="E41" t="n">
-        <v>69000000</v>
+        <v>5.4461321528</v>
       </c>
       <c r="F41" t="n">
-        <v>6882052.659597609</v>
+        <v>0.2821185966637507</v>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Financial Statements</t>
+          <t>Change Ratios</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Inventory (Balance Sheet)</t>
+          <t>Difference in Operating Income Ratio from prior fixed quarter</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>941316423.168898</v>
+        <v>-0.002701132455835906</v>
       </c>
       <c r="C42" t="n">
-        <v>-19626000</v>
+        <v>-7.357101333000001</v>
       </c>
       <c r="D42" t="n">
-        <v>407512500</v>
+        <v>0.001715251300000012</v>
       </c>
       <c r="E42" t="n">
-        <v>8328000000</v>
+        <v>5.2011172407</v>
       </c>
       <c r="F42" t="n">
-        <v>1407393286.129966</v>
+        <v>0.2739475204078941</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Financial Statements</t>
+          <t>Change Ratios</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Inventory (Cash Flow Statement)</t>
+          <t>Difference in Ratio A from prior fixed quarter</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>-10383742.25782035</v>
+        <v>-0.0002139897706401295</v>
       </c>
       <c r="C43" t="n">
-        <v>-420000000</v>
+        <v>-0.1002597382834973</v>
       </c>
       <c r="D43" t="n">
-        <v>0</v>
+        <v>5.387104851526867e-05</v>
       </c>
       <c r="E43" t="n">
-        <v>289000000</v>
+        <v>0.1002597382834973</v>
       </c>
       <c r="F43" t="n">
-        <v>70575014.44370054</v>
+        <v>0.01490370385642221</v>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>Financial Statements</t>
+          <t>Change Ratios</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Investments in Property, Plants, and Equipment</t>
+          <t>Difference in Ratio B from prior fixed quarter</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>-194182976.281852</v>
+        <v>-0.00189503921860355</v>
       </c>
       <c r="C44" t="n">
-        <v>-1921864000</v>
+        <v>-0.5619875314951085</v>
       </c>
       <c r="D44" t="n">
-        <v>-61381500</v>
+        <v>0</v>
       </c>
       <c r="E44" t="n">
-        <v>412700</v>
+        <v>0.5660929836131512</v>
       </c>
       <c r="F44" t="n">
-        <v>313040469.6214882</v>
+        <v>0.04165860202753008</v>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Financial Statements</t>
+          <t>Change Ratios</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Long-Term Debt</t>
+          <t>Difference in Ratio C from prior fixed quarter</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>4157384374.861621</v>
+        <v>-0.007080859118206982</v>
       </c>
       <c r="C45" t="n">
-        <v>-651718</v>
+        <v>-7.766679849278185</v>
       </c>
       <c r="D45" t="n">
-        <v>1828522000</v>
+        <v>0.00718136880629916</v>
       </c>
       <c r="E45" t="n">
-        <v>31359000000</v>
+        <v>7.150002953483518</v>
       </c>
       <c r="F45" t="n">
-        <v>5563500112.275578</v>
+        <v>0.565610782661455</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Financial Statements</t>
+          <t>Change Ratios</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Long-Term Investments</t>
+          <t>Difference in Ratio D from prior fixed quarter</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>493613595.9693735</v>
+        <v>-0.001217753556313899</v>
       </c>
       <c r="C46" t="n">
-        <v>-490677000</v>
+        <v>-0.5702921164457316</v>
       </c>
       <c r="D46" t="n">
-        <v>12732500</v>
+        <v>0</v>
       </c>
       <c r="E46" t="n">
-        <v>10981000000</v>
+        <v>0.5996550622397933</v>
       </c>
       <c r="F46" t="n">
-        <v>1369480812.677983</v>
+        <v>0.0511629411956209</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Financial Statements</t>
+          <t>Change Ratios</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Minority Interest</t>
+          <t>Difference in Ratio E from prior fixed quarter</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>92264442.06086527</v>
+        <v>0.001251291240687483</v>
       </c>
       <c r="C47" t="n">
-        <v>-20252654.038301</v>
+        <v>-0.7967075403567399</v>
       </c>
       <c r="D47" t="n">
-        <v>1759000</v>
+        <v>0.001875234818818239</v>
       </c>
       <c r="E47" t="n">
-        <v>2316406000</v>
+        <v>0.9778573070587835</v>
       </c>
       <c r="F47" t="n">
-        <v>270956746.4137581</v>
+        <v>0.06561942132259552</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Financial Statements</t>
+          <t>Change Ratios</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Net Acquisitions</t>
+          <t>Accounts Payable (Balance Sheet)</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>-32625967.26303927</v>
+        <v>957290323.9327325</v>
       </c>
       <c r="C48" t="n">
-        <v>-805960000</v>
+        <v>-237651171</v>
       </c>
       <c r="D48" t="n">
-        <v>0</v>
+        <v>356700000</v>
       </c>
       <c r="E48" t="n">
-        <v>249000000</v>
+        <v>11433000000</v>
       </c>
       <c r="F48" t="n">
-        <v>115701304.2124059</v>
+        <v>1551108353.022384</v>
       </c>
       <c r="G48" t="inlineStr">
         <is>
@@ -1742,23 +1742,23 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Net Cash Provided by Operating Activities</t>
+          <t>Accounts Payable (Cash Flow Statement)</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>354893994.4036251</v>
+        <v>5154565.153769648</v>
       </c>
       <c r="C49" t="n">
-        <v>-179404000</v>
+        <v>-321769000</v>
       </c>
       <c r="D49" t="n">
-        <v>144174000</v>
+        <v>0</v>
       </c>
       <c r="E49" t="n">
-        <v>3870000000</v>
+        <v>1789652000</v>
       </c>
       <c r="F49" t="n">
-        <v>549880984.747296</v>
+        <v>82110968.90769444</v>
       </c>
       <c r="G49" t="inlineStr">
         <is>
@@ -1769,23 +1769,23 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Net Cash Used for Investing Activities</t>
+          <t>Accounts Receivables</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>-253339898.4697658</v>
+        <v>-11478236.24805989</v>
       </c>
       <c r="C50" t="n">
-        <v>-2840033000</v>
+        <v>-544000000</v>
       </c>
       <c r="D50" t="n">
-        <v>-71524000</v>
+        <v>0</v>
       </c>
       <c r="E50" t="n">
-        <v>325900000</v>
+        <v>325000000</v>
       </c>
       <c r="F50" t="n">
-        <v>444328516.7231604</v>
+        <v>91535961.30454673</v>
       </c>
       <c r="G50" t="inlineStr">
         <is>
@@ -1796,23 +1796,23 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Net Cash Used or Provided by Financing Activities</t>
+          <t>Accumulated Other Comprehensive Income (Loss)</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>-116189055.6289287</v>
+        <v>-404483300.2212174</v>
       </c>
       <c r="C51" t="n">
-        <v>-2444000000</v>
+        <v>-5290000000</v>
       </c>
       <c r="D51" t="n">
-        <v>-29317500</v>
+        <v>-77514000</v>
       </c>
       <c r="E51" t="n">
-        <v>1094000000</v>
+        <v>431595000</v>
       </c>
       <c r="F51" t="n">
-        <v>399791510.5995055</v>
+        <v>874353108.4125022</v>
       </c>
       <c r="G51" t="inlineStr">
         <is>
@@ -1823,23 +1823,23 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Net Change in Cash</t>
+          <t>Capital Expenditure</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>4919539.313980402</v>
+        <v>-192514484.4728179</v>
       </c>
       <c r="C52" t="n">
-        <v>-1161000000</v>
+        <v>-1867000000</v>
       </c>
       <c r="D52" t="n">
-        <v>439500</v>
+        <v>-60129000</v>
       </c>
       <c r="E52" t="n">
-        <v>1401000000</v>
+        <v>412700</v>
       </c>
       <c r="F52" t="n">
-        <v>269603027.0669032</v>
+        <v>310057440.266418</v>
       </c>
       <c r="G52" t="inlineStr">
         <is>
@@ -1850,23 +1850,23 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Net Debt</t>
+          <t>Capital Lease Obligations</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>3582100670.969635</v>
+        <v>24642498.78788461</v>
       </c>
       <c r="C53" t="n">
-        <v>-1044500000</v>
+        <v>0</v>
       </c>
       <c r="D53" t="n">
-        <v>1498679500</v>
+        <v>0</v>
       </c>
       <c r="E53" t="n">
-        <v>30761000000</v>
+        <v>9056234000</v>
       </c>
       <c r="F53" t="n">
-        <v>5313477844.986021</v>
+        <v>228328885.1839498</v>
       </c>
       <c r="G53" t="inlineStr">
         <is>
@@ -1877,23 +1877,23 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Net Income (Cash Flow Statement)</t>
+          <t>Cash and Cash Equivalents</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>189838210.1853327</v>
+        <v>862135865.0702256</v>
       </c>
       <c r="C54" t="n">
-        <v>-327000000</v>
+        <v>0</v>
       </c>
       <c r="D54" t="n">
-        <v>66869500</v>
+        <v>333000000</v>
       </c>
       <c r="E54" t="n">
-        <v>2402000000</v>
+        <v>9223000000</v>
       </c>
       <c r="F54" t="n">
-        <v>337034710.2151847</v>
+        <v>1366595243.166014</v>
       </c>
       <c r="G54" t="inlineStr">
         <is>
@@ -1904,23 +1904,23 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Net Income (Income Statement)</t>
+          <t>Cash and Short Term Investments</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>186964309.9342815</v>
+        <v>1060086810.635769</v>
       </c>
       <c r="C55" t="n">
-        <v>-329864000</v>
+        <v>0</v>
       </c>
       <c r="D55" t="n">
-        <v>67050000</v>
+        <v>363008000</v>
       </c>
       <c r="E55" t="n">
-        <v>2340000000</v>
+        <v>15601000000</v>
       </c>
       <c r="F55" t="n">
-        <v>332573670.1831773</v>
+        <v>1890682420.930147</v>
       </c>
       <c r="G55" t="inlineStr">
         <is>
@@ -1931,23 +1931,23 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Net Income Ratio</t>
+          <t>Cash at Beginning of Period</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>0.0503397518975485</v>
+        <v>867410489.8226552</v>
       </c>
       <c r="C56" t="n">
-        <v>-8.8819426336</v>
+        <v>-2556000</v>
       </c>
       <c r="D56" t="n">
-        <v>0.06586226135000001</v>
+        <v>334000000</v>
       </c>
       <c r="E56" t="n">
-        <v>2.7192118227</v>
+        <v>9610000000</v>
       </c>
       <c r="F56" t="n">
-        <v>0.2915498888197004</v>
+        <v>1388834800.132886</v>
       </c>
       <c r="G56" t="inlineStr">
         <is>
@@ -1958,23 +1958,23 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Net Property Plant Equipment</t>
+          <t>Cash at End of Period</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>4946156314.305075</v>
+        <v>871017693.3940594</v>
       </c>
       <c r="C57" t="n">
-        <v>0</v>
+        <v>-154400</v>
       </c>
       <c r="D57" t="n">
-        <v>1413197500</v>
+        <v>335469000</v>
       </c>
       <c r="E57" t="n">
-        <v>44441000000</v>
+        <v>9743000000</v>
       </c>
       <c r="F57" t="n">
-        <v>7878581995.750476</v>
+        <v>1394641397.299426</v>
       </c>
       <c r="G57" t="inlineStr">
         <is>
@@ -1985,23 +1985,23 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Net Receivables</t>
+          <t>Change in Working Capital</t>
         </is>
       </c>
       <c r="B58" t="n">
-        <v>1283363100.041589</v>
+        <v>-17557103.19706976</v>
       </c>
       <c r="C58" t="n">
-        <v>-4199600</v>
+        <v>-870000000</v>
       </c>
       <c r="D58" t="n">
-        <v>569700000</v>
+        <v>-2384000</v>
       </c>
       <c r="E58" t="n">
-        <v>12146000000</v>
+        <v>753000000</v>
       </c>
       <c r="F58" t="n">
-        <v>1794448777.745643</v>
+        <v>183788257.04855</v>
       </c>
       <c r="G58" t="inlineStr">
         <is>
@@ -2012,23 +2012,23 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Non-Current Deferred Revenue</t>
+          <t>Common Stock</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>248223425.6340992</v>
+        <v>329277684.3612376</v>
       </c>
       <c r="C59" t="n">
-        <v>-500933000</v>
+        <v>-539800</v>
       </c>
       <c r="D59" t="n">
-        <v>0</v>
+        <v>3800000</v>
       </c>
       <c r="E59" t="n">
-        <v>5778000000</v>
+        <v>9817134000</v>
       </c>
       <c r="F59" t="n">
-        <v>725439952.220749</v>
+        <v>925626949.1996731</v>
       </c>
       <c r="G59" t="inlineStr">
         <is>
@@ -2039,23 +2039,23 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Non-Current Deferred Tax Liabilities</t>
+          <t>Common Stock Issued</t>
         </is>
       </c>
       <c r="B60" t="n">
-        <v>704046356.9237548</v>
+        <v>44672509.35733256</v>
       </c>
       <c r="C60" t="n">
-        <v>-3818507</v>
+        <v>-3572000</v>
       </c>
       <c r="D60" t="n">
-        <v>137248500</v>
+        <v>43000</v>
       </c>
       <c r="E60" t="n">
-        <v>8306000000</v>
+        <v>1111490728</v>
       </c>
       <c r="F60" t="n">
-        <v>1394360238.891871</v>
+        <v>124027450.2013901</v>
       </c>
       <c r="G60" t="inlineStr">
         <is>
@@ -2066,23 +2066,23 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Operating Cash Flow</t>
+          <t>Common Stock Repurchased</t>
         </is>
       </c>
       <c r="B61" t="n">
-        <v>354893994.4036251</v>
+        <v>-78527033.89660616</v>
       </c>
       <c r="C61" t="n">
-        <v>-179404000</v>
+        <v>-2086545366</v>
       </c>
       <c r="D61" t="n">
-        <v>144174000</v>
+        <v>-773000</v>
       </c>
       <c r="E61" t="n">
-        <v>3870000000</v>
+        <v>545656614.524539</v>
       </c>
       <c r="F61" t="n">
-        <v>549880984.747296</v>
+        <v>188219352.3448941</v>
       </c>
       <c r="G61" t="inlineStr">
         <is>
@@ -2093,23 +2093,23 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Operating Expenses</t>
+          <t>Cost and Expenses</t>
         </is>
       </c>
       <c r="B62" t="n">
-        <v>546048778.2601695</v>
+        <v>2317513877.074687</v>
       </c>
       <c r="C62" t="n">
-        <v>-13530000</v>
+        <v>-2495000</v>
       </c>
       <c r="D62" t="n">
-        <v>222695500</v>
+        <v>1121064000</v>
       </c>
       <c r="E62" t="n">
-        <v>6252000000</v>
+        <v>22769000000</v>
       </c>
       <c r="F62" t="n">
-        <v>932339076.1354781</v>
+        <v>3357899606.575489</v>
       </c>
       <c r="G62" t="inlineStr">
         <is>
@@ -2120,23 +2120,23 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Operating Income</t>
+          <t>Cost of Revenue</t>
         </is>
       </c>
       <c r="B63" t="n">
-        <v>302408763.0123758</v>
+        <v>1624233369.179577</v>
       </c>
       <c r="C63" t="n">
-        <v>-208377000</v>
+        <v>-3094000</v>
       </c>
       <c r="D63" t="n">
-        <v>123446500</v>
+        <v>787700000</v>
       </c>
       <c r="E63" t="n">
-        <v>3294000000</v>
+        <v>18303000000</v>
       </c>
       <c r="F63" t="n">
-        <v>472764842.777743</v>
+        <v>2405765370.433056</v>
       </c>
       <c r="G63" t="inlineStr">
         <is>
@@ -2147,23 +2147,23 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Operating Income Ratio</t>
+          <t>Debt Repayment</t>
         </is>
       </c>
       <c r="B64" t="n">
-        <v>0.1058576498163668</v>
+        <v>-247880234.2441134</v>
       </c>
       <c r="C64" t="n">
-        <v>-9.7135919166</v>
+        <v>-3001000000</v>
       </c>
       <c r="D64" t="n">
-        <v>0.11759992255</v>
+        <v>-33400000</v>
       </c>
       <c r="E64" t="n">
-        <v>2.8637438343</v>
+        <v>200</v>
       </c>
       <c r="F64" t="n">
-        <v>0.3105883718759841</v>
+        <v>471724050.3716313</v>
       </c>
       <c r="G64" t="inlineStr">
         <is>
@@ -2174,23 +2174,23 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Other Assets</t>
+          <t>Deferred Income Tax</t>
         </is>
       </c>
       <c r="B65" t="n">
-        <v>6824.880599647056</v>
+        <v>6154669.537851976</v>
       </c>
       <c r="C65" t="n">
-        <v>-19834700</v>
+        <v>-253000000</v>
       </c>
       <c r="D65" t="n">
-        <v>0</v>
+        <v>64000</v>
       </c>
       <c r="E65" t="n">
-        <v>8948000</v>
+        <v>1850454000</v>
       </c>
       <c r="F65" t="n">
-        <v>427499.4443150864</v>
+        <v>58927713.28293461</v>
       </c>
       <c r="G65" t="inlineStr">
         <is>
@@ -2201,23 +2201,23 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Other Current Assets</t>
+          <t>Deferred Revenue</t>
         </is>
       </c>
       <c r="B66" t="n">
-        <v>371170937.9799585</v>
+        <v>310000739.6631016</v>
       </c>
       <c r="C66" t="n">
-        <v>-98000</v>
+        <v>-116912000</v>
       </c>
       <c r="D66" t="n">
-        <v>120313000</v>
+        <v>50066000</v>
       </c>
       <c r="E66" t="n">
-        <v>4968950000</v>
+        <v>4918100000</v>
       </c>
       <c r="F66" t="n">
-        <v>665138617.208887</v>
+        <v>642489899.3055267</v>
       </c>
       <c r="G66" t="inlineStr">
         <is>
@@ -2228,23 +2228,23 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Other Current Liabilities</t>
+          <t>Depreciation and Amortization (Cash Flow Statement)</t>
         </is>
       </c>
       <c r="B67" t="n">
-        <v>971625467.1177772</v>
+        <v>141811048.1428043</v>
       </c>
       <c r="C67" t="n">
-        <v>-48317000</v>
+        <v>-675312</v>
       </c>
       <c r="D67" t="n">
-        <v>326047500</v>
+        <v>53551000</v>
       </c>
       <c r="E67" t="n">
-        <v>12137000000</v>
+        <v>1529000000</v>
       </c>
       <c r="F67" t="n">
-        <v>1812385139.722118</v>
+        <v>210315836.1796997</v>
       </c>
       <c r="G67" t="inlineStr">
         <is>
@@ -2255,23 +2255,23 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Other Expenses</t>
+          <t>Depreciation and Amortization (Income Statement)</t>
         </is>
       </c>
       <c r="B68" t="n">
-        <v>50748275.86117355</v>
+        <v>140571212.8343998</v>
       </c>
       <c r="C68" t="n">
-        <v>-64000000</v>
+        <v>-1550000</v>
       </c>
       <c r="D68" t="n">
-        <v>571500</v>
+        <v>54507000</v>
       </c>
       <c r="E68" t="n">
-        <v>16189674590</v>
+        <v>1371000000</v>
       </c>
       <c r="F68" t="n">
-        <v>338468185.6508188</v>
+        <v>203167331.4389332</v>
       </c>
       <c r="G68" t="inlineStr">
         <is>
@@ -2282,23 +2282,23 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Other Financing Activities</t>
+          <t>Diluted EPS</t>
         </is>
       </c>
       <c r="B69" t="n">
-        <v>216082622.684779</v>
+        <v>0.5112486839716827</v>
       </c>
       <c r="C69" t="n">
-        <v>-975168999</v>
+        <v>-156.36</v>
       </c>
       <c r="D69" t="n">
-        <v>8000000</v>
+        <v>0.51</v>
       </c>
       <c r="E69" t="n">
-        <v>3297501000</v>
+        <v>49.73</v>
       </c>
       <c r="F69" t="n">
-        <v>513442205.8098591</v>
+        <v>3.306147260720319</v>
       </c>
       <c r="G69" t="inlineStr">
         <is>
@@ -2309,23 +2309,23 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Other Investing Activities</t>
+          <t>Dividends Paid</t>
         </is>
       </c>
       <c r="B70" t="n">
-        <v>4846309.092750786</v>
+        <v>-91357096.75646824</v>
       </c>
       <c r="C70" t="n">
-        <v>-448000000</v>
+        <v>-1233000000</v>
       </c>
       <c r="D70" t="n">
-        <v>108000</v>
+        <v>-21054000</v>
       </c>
       <c r="E70" t="n">
-        <v>3060433659</v>
+        <v>0</v>
       </c>
       <c r="F70" t="n">
-        <v>96863864.12004521</v>
+        <v>182429714.5518515</v>
       </c>
       <c r="G70" t="inlineStr">
         <is>
@@ -2336,23 +2336,23 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Other Liabilities</t>
+          <t>EBITDA</t>
         </is>
       </c>
       <c r="B71" t="n">
-        <v>101452.4343915341</v>
+        <v>444995396.8195523</v>
       </c>
       <c r="C71" t="n">
-        <v>-3063000</v>
+        <v>-66200000</v>
       </c>
       <c r="D71" t="n">
-        <v>0</v>
+        <v>193000000</v>
       </c>
       <c r="E71" t="n">
-        <v>51076000</v>
+        <v>4410000000</v>
       </c>
       <c r="F71" t="n">
-        <v>2036383.741584519</v>
+        <v>644706471.6177711</v>
       </c>
       <c r="G71" t="inlineStr">
         <is>
@@ -2363,23 +2363,23 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Other Non-Cash Items</t>
+          <t>EBITDA Ratio</t>
         </is>
       </c>
       <c r="B72" t="n">
-        <v>15426331.86512952</v>
+        <v>0.2011604356140134</v>
       </c>
       <c r="C72" t="n">
-        <v>-1848719007</v>
+        <v>-5.769041769</v>
       </c>
       <c r="D72" t="n">
-        <v>1600000</v>
+        <v>0.1724345887</v>
       </c>
       <c r="E72" t="n">
-        <v>703000000</v>
+        <v>2.1555001457</v>
       </c>
       <c r="F72" t="n">
-        <v>109962680.1130758</v>
+        <v>0.2182333179007997</v>
       </c>
       <c r="G72" t="inlineStr">
         <is>
@@ -2390,23 +2390,23 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Other Non-Current Assets</t>
+          <t>EPS</t>
         </is>
       </c>
       <c r="B73" t="n">
-        <v>506812134.3714845</v>
+        <v>0.5243659466327827</v>
       </c>
       <c r="C73" t="n">
-        <v>-75012534818</v>
+        <v>-156.36</v>
       </c>
       <c r="D73" t="n">
-        <v>160004000</v>
+        <v>0.52</v>
       </c>
       <c r="E73" t="n">
-        <v>8037000000</v>
+        <v>53.75</v>
       </c>
       <c r="F73" t="n">
-        <v>1760996004.388484</v>
+        <v>3.331950797510649</v>
       </c>
       <c r="G73" t="inlineStr">
         <is>
@@ -2417,23 +2417,23 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Other Non-Current Liabilities</t>
+          <t>Effect of Foreign Exchange Changes on Cash</t>
         </is>
       </c>
       <c r="B74" t="n">
-        <v>977014033.7578533</v>
+        <v>-1697085.834271657</v>
       </c>
       <c r="C74" t="n">
-        <v>-286041895</v>
+        <v>-65000000</v>
       </c>
       <c r="D74" t="n">
-        <v>328324500</v>
+        <v>0</v>
       </c>
       <c r="E74" t="n">
-        <v>11890564000</v>
+        <v>52000000</v>
       </c>
       <c r="F74" t="n">
-        <v>1685843225.830824</v>
+        <v>11200007.88258313</v>
       </c>
       <c r="G74" t="inlineStr">
         <is>
@@ -2444,23 +2444,23 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Other Total Stockholders' Equity</t>
+          <t>Free Cash Flow</t>
         </is>
       </c>
       <c r="B75" t="n">
-        <v>1130983775.667672</v>
+        <v>156892657.8145959</v>
       </c>
       <c r="C75" t="n">
-        <v>-12393000000</v>
+        <v>-541000000</v>
       </c>
       <c r="D75" t="n">
-        <v>421317000</v>
+        <v>51691000</v>
       </c>
       <c r="E75" t="n">
-        <v>34030400000</v>
+        <v>2683000000</v>
       </c>
       <c r="F75" t="n">
-        <v>3589780224.867846</v>
+        <v>389666937.1908457</v>
       </c>
       <c r="G75" t="inlineStr">
         <is>
@@ -2471,23 +2471,23 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Other Working Capital</t>
+          <t>General and Administrative Expenses</t>
         </is>
       </c>
       <c r="B76" t="n">
-        <v>21147653.9827458</v>
+        <v>153933016.9881425</v>
       </c>
       <c r="C76" t="n">
-        <v>-1788851160</v>
+        <v>-2738500</v>
       </c>
       <c r="D76" t="n">
-        <v>0</v>
+        <v>33768000</v>
       </c>
       <c r="E76" t="n">
-        <v>40341689407</v>
+        <v>2007000000</v>
       </c>
       <c r="F76" t="n">
-        <v>775619463.2611961</v>
+        <v>303900948.3754831</v>
       </c>
       <c r="G76" t="inlineStr">
         <is>
@@ -2498,23 +2498,23 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Preferred Stock</t>
+          <t>Goodwill</t>
         </is>
       </c>
       <c r="B77" t="n">
-        <v>9365360.698996564</v>
+        <v>2009260205.056044</v>
       </c>
       <c r="C77" t="n">
-        <v>0</v>
+        <v>-202702100</v>
       </c>
       <c r="D77" t="n">
-        <v>0</v>
+        <v>636039000</v>
       </c>
       <c r="E77" t="n">
-        <v>401500000</v>
+        <v>23389000000</v>
       </c>
       <c r="F77" t="n">
-        <v>42432348.3748346</v>
+        <v>3554057246.391675</v>
       </c>
       <c r="G77" t="inlineStr">
         <is>
@@ -2525,23 +2525,23 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Purchases of Investments</t>
+          <t>Goodwill and Intangible Assets</t>
         </is>
       </c>
       <c r="B78" t="n">
-        <v>-102973220.3364844</v>
+        <v>3102882804.880267</v>
       </c>
       <c r="C78" t="n">
-        <v>-11997654000</v>
+        <v>-1618944000</v>
       </c>
       <c r="D78" t="n">
-        <v>0</v>
+        <v>970000000</v>
       </c>
       <c r="E78" t="n">
-        <v>81823000</v>
+        <v>37123000000</v>
       </c>
       <c r="F78" t="n">
-        <v>344612110.0478056</v>
+        <v>5639038312.523863</v>
       </c>
       <c r="G78" t="inlineStr">
         <is>
@@ -2552,23 +2552,23 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Research and Development Expenses</t>
+          <t>Gross Profit</t>
         </is>
       </c>
       <c r="B79" t="n">
-        <v>27530996.49700176</v>
+        <v>861821178.0733739</v>
       </c>
       <c r="C79" t="n">
-        <v>-214000</v>
+        <v>-7195000</v>
       </c>
       <c r="D79" t="n">
-        <v>0</v>
+        <v>378500000</v>
       </c>
       <c r="E79" t="n">
-        <v>893000000</v>
+        <v>9223000000</v>
       </c>
       <c r="F79" t="n">
-        <v>93165301.96150617</v>
+        <v>1365410717.452004</v>
       </c>
       <c r="G79" t="inlineStr">
         <is>
@@ -2579,23 +2579,23 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Retained Earnings</t>
+          <t>Gross Profit Ratio</t>
         </is>
       </c>
       <c r="B80" t="n">
-        <v>3643670803.878135</v>
+        <v>0.3683520444749319</v>
       </c>
       <c r="C80" t="n">
-        <v>-4839000000</v>
+        <v>-5.6527436527</v>
       </c>
       <c r="D80" t="n">
-        <v>1300015500</v>
+        <v>0.3430254656</v>
       </c>
       <c r="E80" t="n">
-        <v>37899000000</v>
+        <v>2.3163345465</v>
       </c>
       <c r="F80" t="n">
-        <v>6417848831.202461</v>
+        <v>0.2633712166038495</v>
       </c>
       <c r="G80" t="inlineStr">
         <is>
@@ -2606,23 +2606,23 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Revenue</t>
+          <t>Income Before Tax</t>
         </is>
       </c>
       <c r="B81" t="n">
-        <v>2763740179.564392</v>
+        <v>255351974.5348443</v>
       </c>
       <c r="C81" t="n">
-        <v>-4273000</v>
+        <v>-353153000</v>
       </c>
       <c r="D81" t="n">
-        <v>1308000000</v>
+        <v>91900000</v>
       </c>
       <c r="E81" t="n">
-        <v>25420000000</v>
+        <v>2951000000</v>
       </c>
       <c r="F81" t="n">
-        <v>4026578837.743789</v>
+        <v>434623029.4258907</v>
       </c>
       <c r="G81" t="inlineStr">
         <is>
@@ -2633,23 +2633,23 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Sales and Maturities of Investments</t>
+          <t>Income Before Tax Ratio</t>
         </is>
       </c>
       <c r="B82" t="n">
-        <v>97797529.17000552</v>
+        <v>0.07174942881573788</v>
       </c>
       <c r="C82" t="n">
-        <v>-9409000</v>
+        <v>-9.3813885267</v>
       </c>
       <c r="D82" t="n">
-        <v>0</v>
+        <v>0.09295742880000001</v>
       </c>
       <c r="E82" t="n">
-        <v>8936406000</v>
+        <v>2.678365705</v>
       </c>
       <c r="F82" t="n">
-        <v>307975538.5106821</v>
+        <v>0.3498729494382256</v>
       </c>
       <c r="G82" t="inlineStr">
         <is>
@@ -2660,23 +2660,23 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Selling General and Administrative Expenses</t>
+          <t>Income Tax Expense</t>
         </is>
       </c>
       <c r="B83" t="n">
-        <v>300347623.8613659</v>
+        <v>69444774.32509148</v>
       </c>
       <c r="C83" t="n">
-        <v>-5054000</v>
+        <v>-119131000</v>
       </c>
       <c r="D83" t="n">
-        <v>120995500</v>
+        <v>22100000</v>
       </c>
       <c r="E83" t="n">
-        <v>3343000000</v>
+        <v>736000000</v>
       </c>
       <c r="F83" t="n">
-        <v>491028139.5322289</v>
+        <v>121681731.4320157</v>
       </c>
       <c r="G83" t="inlineStr">
         <is>
@@ -2687,23 +2687,23 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Selling and Marketing Expenses</t>
+          <t>Intangible Assets</t>
         </is>
       </c>
       <c r="B84" t="n">
-        <v>25644369.53880071</v>
+        <v>835940509.5094651</v>
       </c>
       <c r="C84" t="n">
-        <v>-3003000</v>
+        <v>-421000</v>
       </c>
       <c r="D84" t="n">
-        <v>0</v>
+        <v>170197000</v>
       </c>
       <c r="E84" t="n">
-        <v>876761000</v>
+        <v>14110100000</v>
       </c>
       <c r="F84" t="n">
-        <v>99025764.5581083</v>
+        <v>1785542119.17041</v>
       </c>
       <c r="G84" t="inlineStr">
         <is>
@@ -2714,23 +2714,23 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Short Term Investments</t>
+          <t>Interest Expense</t>
         </is>
       </c>
       <c r="B85" t="n">
-        <v>178641675.1468396</v>
+        <v>46568508.69498868</v>
       </c>
       <c r="C85" t="n">
-        <v>-515000</v>
+        <v>-16400000</v>
       </c>
       <c r="D85" t="n">
-        <v>0</v>
+        <v>23000000</v>
       </c>
       <c r="E85" t="n">
-        <v>6178000000</v>
+        <v>386000000</v>
       </c>
       <c r="F85" t="n">
-        <v>590076249.1642418</v>
+        <v>61712161.15251228</v>
       </c>
       <c r="G85" t="inlineStr">
         <is>
@@ -2741,23 +2741,23 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Short-Term Debt</t>
+          <t>Interest Income</t>
         </is>
       </c>
       <c r="B86" t="n">
-        <v>464412829.9749784</v>
+        <v>2372725.227711567</v>
       </c>
       <c r="C86" t="n">
-        <v>-655561</v>
+        <v>-62900</v>
       </c>
       <c r="D86" t="n">
-        <v>83408000</v>
+        <v>0</v>
       </c>
       <c r="E86" t="n">
-        <v>5363000000</v>
+        <v>69000000</v>
       </c>
       <c r="F86" t="n">
-        <v>881907750.8517716</v>
+        <v>6859086.749159348</v>
       </c>
       <c r="G86" t="inlineStr">
         <is>
@@ -2768,23 +2768,23 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Stock-Based Compensation</t>
+          <t>Inventory (Balance Sheet)</t>
         </is>
       </c>
       <c r="B87" t="n">
-        <v>14543170.39325017</v>
+        <v>933043177.3951372</v>
       </c>
       <c r="C87" t="n">
-        <v>-36000000</v>
+        <v>-19626000</v>
       </c>
       <c r="D87" t="n">
-        <v>5100000</v>
+        <v>403789000</v>
       </c>
       <c r="E87" t="n">
-        <v>254000000</v>
+        <v>8328000000</v>
       </c>
       <c r="F87" t="n">
-        <v>30176788.95257358</v>
+        <v>1398934358.21151</v>
       </c>
       <c r="G87" t="inlineStr">
         <is>
@@ -2795,23 +2795,23 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Tax Assets</t>
+          <t>Inventory (Cash Flow Statement)</t>
         </is>
       </c>
       <c r="B88" t="n">
-        <v>376499884.6999475</v>
+        <v>-10302495.14167652</v>
       </c>
       <c r="C88" t="n">
-        <v>-2310712000</v>
+        <v>-420000000</v>
       </c>
       <c r="D88" t="n">
-        <v>49195000</v>
+        <v>0</v>
       </c>
       <c r="E88" t="n">
-        <v>6535000000</v>
+        <v>289000000</v>
       </c>
       <c r="F88" t="n">
-        <v>902752313.0390466</v>
+        <v>70374129.31851257</v>
       </c>
       <c r="G88" t="inlineStr">
         <is>
@@ -2822,23 +2822,23 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Tax Payable</t>
+          <t>Investments in Property, Plants, and Equipment</t>
         </is>
       </c>
       <c r="B89" t="n">
-        <v>61484524.50367177</v>
+        <v>-193897744.953849</v>
       </c>
       <c r="C89" t="n">
-        <v>-87400</v>
+        <v>-1921864000</v>
       </c>
       <c r="D89" t="n">
-        <v>2828000</v>
+        <v>-60373000</v>
       </c>
       <c r="E89" t="n">
-        <v>1187000000</v>
+        <v>412700</v>
       </c>
       <c r="F89" t="n">
-        <v>152142261.8459613</v>
+        <v>313436441.141196</v>
       </c>
       <c r="G89" t="inlineStr">
         <is>
@@ -2849,23 +2849,23 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Total Assets</t>
+          <t>Long-Term Debt</t>
         </is>
       </c>
       <c r="B90" t="n">
-        <v>15623432251.62567</v>
+        <v>4159473460.267453</v>
       </c>
       <c r="C90" t="n">
-        <v>123279</v>
+        <v>-651718</v>
       </c>
       <c r="D90" t="n">
-        <v>7059132500</v>
+        <v>1822139000</v>
       </c>
       <c r="E90" t="n">
-        <v>131556000000</v>
+        <v>31359000000</v>
       </c>
       <c r="F90" t="n">
-        <v>21907186479.14707</v>
+        <v>5574538232.320455</v>
       </c>
       <c r="G90" t="inlineStr">
         <is>
@@ -2876,23 +2876,23 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Total Current Assets</t>
+          <t>Long-Term Investments</t>
         </is>
       </c>
       <c r="B91" t="n">
-        <v>3959899836.063107</v>
+        <v>494196440.4129025</v>
       </c>
       <c r="C91" t="n">
-        <v>29954</v>
+        <v>-490677000</v>
       </c>
       <c r="D91" t="n">
-        <v>1936936500</v>
+        <v>12449000</v>
       </c>
       <c r="E91" t="n">
-        <v>41276000000</v>
+        <v>10981000000</v>
       </c>
       <c r="F91" t="n">
-        <v>5741692814.20156</v>
+        <v>1359571399.495756</v>
       </c>
       <c r="G91" t="inlineStr">
         <is>
@@ -2903,23 +2903,23 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Total Current Liabilities</t>
+          <t>Minority Interest</t>
         </is>
       </c>
       <c r="B92" t="n">
-        <v>2835208388.078846</v>
+        <v>90043651.06781109</v>
       </c>
       <c r="C92" t="n">
-        <v>12178</v>
+        <v>-20252654.038301</v>
       </c>
       <c r="D92" t="n">
-        <v>1142000000</v>
+        <v>1600000</v>
       </c>
       <c r="E92" t="n">
-        <v>29919000000</v>
+        <v>2316406000</v>
       </c>
       <c r="F92" t="n">
-        <v>4276706355.299355</v>
+        <v>268200905.9280031</v>
       </c>
       <c r="G92" t="inlineStr">
         <is>
@@ -2930,23 +2930,23 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Total Debt</t>
+          <t>Net Acquisitions</t>
         </is>
       </c>
       <c r="B93" t="n">
-        <v>4591360324.251768</v>
+        <v>-32878764.1838303</v>
       </c>
       <c r="C93" t="n">
+        <v>-805960000</v>
+      </c>
+      <c r="D93" t="n">
         <v>0</v>
       </c>
-      <c r="D93" t="n">
-        <v>2025288000</v>
-      </c>
       <c r="E93" t="n">
-        <v>37124000000</v>
+        <v>249000000</v>
       </c>
       <c r="F93" t="n">
-        <v>6242100940.739635</v>
+        <v>116107004.1970539</v>
       </c>
       <c r="G93" t="inlineStr">
         <is>
@@ -2957,23 +2957,23 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Total Equity</t>
+          <t>Net Cash Provided by Operating Activities</t>
         </is>
       </c>
       <c r="B94" t="n">
-        <v>4987498022.074237</v>
+        <v>352446106.8143697</v>
       </c>
       <c r="C94" t="n">
-        <v>-501467000</v>
+        <v>-179404000</v>
       </c>
       <c r="D94" t="n">
-        <v>2115000000</v>
+        <v>143626000</v>
       </c>
       <c r="E94" t="n">
-        <v>49975000000</v>
+        <v>3870000000</v>
       </c>
       <c r="F94" t="n">
-        <v>7273418780.532268</v>
+        <v>545602564.6327243</v>
       </c>
       <c r="G94" t="inlineStr">
         <is>
@@ -2984,23 +2984,23 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Total Investments</t>
+          <t>Net Cash Used for Investing Activities</t>
         </is>
       </c>
       <c r="B95" t="n">
-        <v>728580576.0119803</v>
+        <v>-252575304.4388635</v>
       </c>
       <c r="C95" t="n">
-        <v>-334673000</v>
+        <v>-2840033000</v>
       </c>
       <c r="D95" t="n">
-        <v>42569500</v>
+        <v>-71100000</v>
       </c>
       <c r="E95" t="n">
-        <v>19331000000</v>
+        <v>325900000</v>
       </c>
       <c r="F95" t="n">
-        <v>1963853124.76086</v>
+        <v>443647871.5231475</v>
       </c>
       <c r="G95" t="inlineStr">
         <is>
@@ -3011,23 +3011,23 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Total Liabilities</t>
+          <t>Net Cash Used or Provided by Financing Activities</t>
         </is>
       </c>
       <c r="B96" t="n">
-        <v>9810477769.614729</v>
+        <v>-114570062.0014226</v>
       </c>
       <c r="C96" t="n">
-        <v>79283</v>
+        <v>-2444000000</v>
       </c>
       <c r="D96" t="n">
-        <v>4315644500</v>
+        <v>-29157000</v>
       </c>
       <c r="E96" t="n">
-        <v>87293000000</v>
+        <v>1094000000</v>
       </c>
       <c r="F96" t="n">
-        <v>13464804883.87591</v>
+        <v>399330481.5213416</v>
       </c>
       <c r="G96" t="inlineStr">
         <is>
@@ -3038,23 +3038,23 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Total Liabilities and Stockholders' Equity</t>
+          <t>Net Change in Cash</t>
         </is>
       </c>
       <c r="B97" t="n">
-        <v>15588449533.10715</v>
+        <v>3933018.182767525</v>
       </c>
       <c r="C97" t="n">
-        <v>123279</v>
+        <v>-1161000000</v>
       </c>
       <c r="D97" t="n">
-        <v>7057469000</v>
+        <v>573000</v>
       </c>
       <c r="E97" t="n">
-        <v>131556000000</v>
+        <v>1401000000</v>
       </c>
       <c r="F97" t="n">
-        <v>21902353741.35348</v>
+        <v>269005283.6798655</v>
       </c>
       <c r="G97" t="inlineStr">
         <is>
@@ -3065,23 +3065,23 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Total Liabilities and Total Equity</t>
+          <t>Net Debt</t>
         </is>
       </c>
       <c r="B98" t="n">
-        <v>15588449533.10715</v>
+        <v>3597141664.585124</v>
       </c>
       <c r="C98" t="n">
-        <v>123279</v>
+        <v>-1044500000</v>
       </c>
       <c r="D98" t="n">
-        <v>7057469000</v>
+        <v>1508594000</v>
       </c>
       <c r="E98" t="n">
-        <v>131556000000</v>
+        <v>30761000000</v>
       </c>
       <c r="F98" t="n">
-        <v>21902353741.35348</v>
+        <v>5338457121.62334</v>
       </c>
       <c r="G98" t="inlineStr">
         <is>
@@ -3092,23 +3092,23 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Total Non-Current Assets</t>
+          <t>Net Income (Cash Flow Statement)</t>
         </is>
       </c>
       <c r="B99" t="n">
-        <v>11003567097.66838</v>
+        <v>189122176.1152642</v>
       </c>
       <c r="C99" t="n">
-        <v>49861</v>
+        <v>-327000000</v>
       </c>
       <c r="D99" t="n">
-        <v>4170300000</v>
+        <v>66190000</v>
       </c>
       <c r="E99" t="n">
-        <v>104263000000</v>
+        <v>2402000000</v>
       </c>
       <c r="F99" t="n">
-        <v>15962173630.31497</v>
+        <v>336635167.3495772</v>
       </c>
       <c r="G99" t="inlineStr">
         <is>
@@ -3119,23 +3119,23 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Total Non-Current Liabilities</t>
+          <t>Net Income (Income Statement)</t>
         </is>
       </c>
       <c r="B100" t="n">
-        <v>6631926419.44329</v>
+        <v>185944828.2694118</v>
       </c>
       <c r="C100" t="n">
-        <v>53696</v>
+        <v>-329864000</v>
       </c>
       <c r="D100" t="n">
-        <v>2823750000</v>
+        <v>66389000</v>
       </c>
       <c r="E100" t="n">
-        <v>54300000000</v>
+        <v>2340000000</v>
       </c>
       <c r="F100" t="n">
-        <v>9401594024.196987</v>
+        <v>330952161.4865037</v>
       </c>
       <c r="G100" t="inlineStr">
         <is>
@@ -3146,23 +3146,23 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Total Other Income Expenses Net</t>
+          <t>Net Income Ratio</t>
         </is>
       </c>
       <c r="B101" t="n">
-        <v>-13084263.75792919</v>
+        <v>0.05055366274501725</v>
       </c>
       <c r="C101" t="n">
-        <v>-503976000</v>
+        <v>-8.8819426336</v>
       </c>
       <c r="D101" t="n">
-        <v>-900000</v>
+        <v>0.0661483169</v>
       </c>
       <c r="E101" t="n">
-        <v>286000000</v>
+        <v>2.7192118227</v>
       </c>
       <c r="F101" t="n">
-        <v>72543230.98287372</v>
+        <v>0.2947142455158262</v>
       </c>
       <c r="G101" t="inlineStr">
         <is>
@@ -3173,23 +3173,23 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Total Stockholders' Equity</t>
+          <t>Net Property Plant Equipment</t>
         </is>
       </c>
       <c r="B102" t="n">
-        <v>4949232739.444783</v>
+        <v>4931687321.779444</v>
       </c>
       <c r="C102" t="n">
-        <v>-526491000</v>
+        <v>0</v>
       </c>
       <c r="D102" t="n">
-        <v>2110773500</v>
+        <v>1389600000</v>
       </c>
       <c r="E102" t="n">
-        <v>49269000000</v>
+        <v>44441000000</v>
       </c>
       <c r="F102" t="n">
-        <v>7190925518.026225</v>
+        <v>7885938319.988754</v>
       </c>
       <c r="G102" t="inlineStr">
         <is>
@@ -3200,23 +3200,23 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Weighted Average Shares Outstanding</t>
+          <t>Net Receivables</t>
         </is>
       </c>
       <c r="B103" t="n">
-        <v>355222897.1008818</v>
+        <v>1276905848.629186</v>
       </c>
       <c r="C103" t="n">
-        <v>0</v>
+        <v>-4199600</v>
       </c>
       <c r="D103" t="n">
-        <v>146624411</v>
+        <v>570338000</v>
       </c>
       <c r="E103" t="n">
-        <v>13751391147</v>
+        <v>12116000000</v>
       </c>
       <c r="F103" t="n">
-        <v>727556653.1401314</v>
+        <v>1776578353.433844</v>
       </c>
       <c r="G103" t="inlineStr">
         <is>
@@ -3227,23 +3227,23 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Weighted Average Shares Outstanding (Diluted)</t>
+          <t>Non-Current Deferred Revenue</t>
         </is>
       </c>
       <c r="B104" t="n">
-        <v>318383151.7869489</v>
+        <v>248840448.2323168</v>
       </c>
       <c r="C104" t="n">
+        <v>-500933000</v>
+      </c>
+      <c r="D104" t="n">
         <v>0</v>
       </c>
-      <c r="D104" t="n">
-        <v>146042500</v>
-      </c>
       <c r="E104" t="n">
-        <v>13986214405</v>
+        <v>5778000000</v>
       </c>
       <c r="F104" t="n">
-        <v>548657214.6378666</v>
+        <v>723186467.0083231</v>
       </c>
       <c r="G104" t="inlineStr">
         <is>
@@ -3254,241 +3254,1483 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Market Capitalization</t>
+          <t>Non-Current Deferred Tax Liabilities</t>
         </is>
       </c>
       <c r="B105" t="n">
-        <v>19114488572.95097</v>
+        <v>702874797.7352276</v>
       </c>
       <c r="C105" t="n">
-        <v>106422</v>
+        <v>-3818507</v>
       </c>
       <c r="D105" t="n">
-        <v>6415265242.5</v>
+        <v>135597000</v>
       </c>
       <c r="E105" t="n">
-        <v>726320349360</v>
+        <v>8306000000</v>
       </c>
       <c r="F105" t="n">
-        <v>44481854214.23445</v>
+        <v>1400029509.57056</v>
       </c>
       <c r="G105" t="inlineStr">
         <is>
-          <t>Market Capitalization</t>
+          <t>Financial Statements</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Days Since Call</t>
+          <t>Operating Cash Flow</t>
         </is>
       </c>
       <c r="B106" t="n">
-        <v>58.12574955908289</v>
+        <v>352446106.8143697</v>
       </c>
       <c r="C106" t="n">
-        <v>0</v>
+        <v>-179404000</v>
       </c>
       <c r="D106" t="n">
-        <v>61</v>
+        <v>143626000</v>
       </c>
       <c r="E106" t="n">
-        <v>91</v>
+        <v>3870000000</v>
       </c>
       <c r="F106" t="n">
-        <v>13.42351467622752</v>
+        <v>545602564.6327243</v>
       </c>
       <c r="G106" t="inlineStr">
         <is>
-          <t>Metadata</t>
+          <t>Financial Statements</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>First Principal Component of Tone</t>
+          <t>Operating Expenses</t>
         </is>
       </c>
       <c r="B107" t="n">
-        <v>-0.03133290132296755</v>
+        <v>538189512.4928595</v>
       </c>
       <c r="C107" t="n">
-        <v>-2.912620748125866</v>
+        <v>-13530000</v>
       </c>
       <c r="D107" t="n">
-        <v>-0.2218978763026523</v>
+        <v>221700000</v>
       </c>
       <c r="E107" t="n">
-        <v>25.34829492850656</v>
+        <v>6252000000</v>
       </c>
       <c r="F107" t="n">
-        <v>1.323055126913059</v>
+        <v>918426909.5997303</v>
       </c>
       <c r="G107" t="inlineStr">
         <is>
-          <t>NLP Feature</t>
+          <t>Financial Statements</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Gunning-Fog Score</t>
+          <t>Operating Income</t>
         </is>
       </c>
       <c r="B108" t="n">
-        <v>12.50574628783717</v>
+        <v>302231079.7564144</v>
       </c>
       <c r="C108" t="n">
-        <v>8.551054692434002</v>
+        <v>-208377000</v>
       </c>
       <c r="D108" t="n">
-        <v>12.41789794221181</v>
+        <v>122000000</v>
       </c>
       <c r="E108" t="n">
-        <v>19.28576584705617</v>
+        <v>3294000000</v>
       </c>
       <c r="F108" t="n">
-        <v>1.315881734691042</v>
+        <v>475077278.1518538</v>
       </c>
       <c r="G108" t="inlineStr">
         <is>
-          <t>NLP Feature</t>
+          <t>Financial Statements</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Number of Questions</t>
+          <t>Operating Income Ratio</t>
         </is>
       </c>
       <c r="B109" t="n">
-        <v>36.47231040564374</v>
+        <v>0.1060917269720821</v>
       </c>
       <c r="C109" t="n">
-        <v>0</v>
+        <v>-9.7135919166</v>
       </c>
       <c r="D109" t="n">
-        <v>35</v>
+        <v>0.1178407434</v>
       </c>
       <c r="E109" t="n">
-        <v>107</v>
+        <v>2.8637438343</v>
       </c>
       <c r="F109" t="n">
-        <v>16.37942658425768</v>
+        <v>0.3132517465588101</v>
       </c>
       <c r="G109" t="inlineStr">
         <is>
-          <t>NLP Feature</t>
+          <t>Financial Statements</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Numeric Transparency</t>
+          <t>Other Assets</t>
         </is>
       </c>
       <c r="B110" t="n">
-        <v>0.1223192239858907</v>
+        <v>5662.386277001574</v>
       </c>
       <c r="C110" t="n">
-        <v>0.01</v>
+        <v>-19834700</v>
       </c>
       <c r="D110" t="n">
-        <v>0.12</v>
+        <v>0</v>
       </c>
       <c r="E110" t="n">
-        <v>0.4</v>
+        <v>8948000</v>
       </c>
       <c r="F110" t="n">
-        <v>0.04638530791496485</v>
+        <v>421776.9308215601</v>
       </c>
       <c r="G110" t="inlineStr">
         <is>
-          <t>NLP Feature</t>
+          <t>Financial Statements</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Positivity Score</t>
+          <t>Other Current Assets</t>
         </is>
       </c>
       <c r="B111" t="n">
-        <v>0.186157235324527</v>
+        <v>370526390.8797786</v>
       </c>
       <c r="C111" t="n">
-        <v>-0.2045797968671188</v>
+        <v>-98000</v>
       </c>
       <c r="D111" t="n">
-        <v>0.1813052114249762</v>
+        <v>119600000</v>
       </c>
       <c r="E111" t="n">
-        <v>0.6748757146226736</v>
+        <v>4968950000</v>
       </c>
       <c r="F111" t="n">
-        <v>0.1006535592018803</v>
+        <v>664643317.2146792</v>
       </c>
       <c r="G111" t="inlineStr">
         <is>
-          <t>NLP Feature</t>
+          <t>Financial Statements</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Word Count</t>
+          <t>Other Current Liabilities</t>
         </is>
       </c>
       <c r="B112" t="n">
-        <v>8829.041975308643</v>
+        <v>955075890.9257107</v>
       </c>
       <c r="C112" t="n">
-        <v>525</v>
+        <v>-48317000</v>
       </c>
       <c r="D112" t="n">
-        <v>9080</v>
+        <v>322800000</v>
       </c>
       <c r="E112" t="n">
-        <v>22006</v>
+        <v>12137000000</v>
       </c>
       <c r="F112" t="n">
-        <v>2479.442021941137</v>
+        <v>1782231297.368809</v>
       </c>
       <c r="G112" t="inlineStr">
         <is>
-          <t>NLP Feature</t>
+          <t>Financial Statements</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
+          <t>Other Expenses</t>
+        </is>
+      </c>
+      <c r="B113" t="n">
+        <v>50749806.81579811</v>
+      </c>
+      <c r="C113" t="n">
+        <v>-64000000</v>
+      </c>
+      <c r="D113" t="n">
+        <v>585000</v>
+      </c>
+      <c r="E113" t="n">
+        <v>16189674590</v>
+      </c>
+      <c r="F113" t="n">
+        <v>342110629.6559865</v>
+      </c>
+      <c r="G113" t="inlineStr">
+        <is>
+          <t>Financial Statements</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>Other Financing Activities</t>
+        </is>
+      </c>
+      <c r="B114" t="n">
+        <v>217421866.4217146</v>
+      </c>
+      <c r="C114" t="n">
+        <v>-975168999</v>
+      </c>
+      <c r="D114" t="n">
+        <v>8000000</v>
+      </c>
+      <c r="E114" t="n">
+        <v>3297501000</v>
+      </c>
+      <c r="F114" t="n">
+        <v>515334960.4481803</v>
+      </c>
+      <c r="G114" t="inlineStr">
+        <is>
+          <t>Financial Statements</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>Other Investing Activities</t>
+        </is>
+      </c>
+      <c r="B115" t="n">
+        <v>4573739.093616209</v>
+      </c>
+      <c r="C115" t="n">
+        <v>-448000000</v>
+      </c>
+      <c r="D115" t="n">
+        <v>106000</v>
+      </c>
+      <c r="E115" t="n">
+        <v>3060433659</v>
+      </c>
+      <c r="F115" t="n">
+        <v>96736267.62435009</v>
+      </c>
+      <c r="G115" t="inlineStr">
+        <is>
+          <t>Financial Statements</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>Other Liabilities</t>
+        </is>
+      </c>
+      <c r="B116" t="n">
+        <v>95902.5781448537</v>
+      </c>
+      <c r="C116" t="n">
+        <v>-3063000</v>
+      </c>
+      <c r="D116" t="n">
+        <v>0</v>
+      </c>
+      <c r="E116" t="n">
+        <v>51076000</v>
+      </c>
+      <c r="F116" t="n">
+        <v>1967227.534466839</v>
+      </c>
+      <c r="G116" t="inlineStr">
+        <is>
+          <t>Financial Statements</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>Other Non-Cash Items</t>
+        </is>
+      </c>
+      <c r="B117" t="n">
+        <v>15325139.74636312</v>
+      </c>
+      <c r="C117" t="n">
+        <v>-1848719007</v>
+      </c>
+      <c r="D117" t="n">
+        <v>1621000</v>
+      </c>
+      <c r="E117" t="n">
+        <v>703000000</v>
+      </c>
+      <c r="F117" t="n">
+        <v>109294805.7936874</v>
+      </c>
+      <c r="G117" t="inlineStr">
+        <is>
+          <t>Financial Statements</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>Other Non-Current Assets</t>
+        </is>
+      </c>
+      <c r="B118" t="n">
+        <v>506778121.0381185</v>
+      </c>
+      <c r="C118" t="n">
+        <v>-75012534818</v>
+      </c>
+      <c r="D118" t="n">
+        <v>158696000</v>
+      </c>
+      <c r="E118" t="n">
+        <v>8037000000</v>
+      </c>
+      <c r="F118" t="n">
+        <v>1778143597.093129</v>
+      </c>
+      <c r="G118" t="inlineStr">
+        <is>
+          <t>Financial Statements</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>Other Non-Current Liabilities</t>
+        </is>
+      </c>
+      <c r="B119" t="n">
+        <v>975892048.3889351</v>
+      </c>
+      <c r="C119" t="n">
+        <v>-286041895</v>
+      </c>
+      <c r="D119" t="n">
+        <v>327700000</v>
+      </c>
+      <c r="E119" t="n">
+        <v>11890564000</v>
+      </c>
+      <c r="F119" t="n">
+        <v>1686827873.948477</v>
+      </c>
+      <c r="G119" t="inlineStr">
+        <is>
+          <t>Financial Statements</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>Other Total Stockholders' Equity</t>
+        </is>
+      </c>
+      <c r="B120" t="n">
+        <v>1135331510.721925</v>
+      </c>
+      <c r="C120" t="n">
+        <v>-12393000000</v>
+      </c>
+      <c r="D120" t="n">
+        <v>427000000</v>
+      </c>
+      <c r="E120" t="n">
+        <v>34030400000</v>
+      </c>
+      <c r="F120" t="n">
+        <v>3586435863.553204</v>
+      </c>
+      <c r="G120" t="inlineStr">
+        <is>
+          <t>Financial Statements</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>Other Working Capital</t>
+        </is>
+      </c>
+      <c r="B121" t="n">
+        <v>21414823.22041815</v>
+      </c>
+      <c r="C121" t="n">
+        <v>-1788851160</v>
+      </c>
+      <c r="D121" t="n">
+        <v>0</v>
+      </c>
+      <c r="E121" t="n">
+        <v>40341689407</v>
+      </c>
+      <c r="F121" t="n">
+        <v>786599061.3492982</v>
+      </c>
+      <c r="G121" t="inlineStr">
+        <is>
+          <t>Financial Statements</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>Preferred Stock</t>
+        </is>
+      </c>
+      <c r="B122" t="n">
+        <v>9475146.220663156</v>
+      </c>
+      <c r="C122" t="n">
+        <v>0</v>
+      </c>
+      <c r="D122" t="n">
+        <v>0</v>
+      </c>
+      <c r="E122" t="n">
+        <v>401500000</v>
+      </c>
+      <c r="F122" t="n">
+        <v>42785110.93042695</v>
+      </c>
+      <c r="G122" t="inlineStr">
+        <is>
+          <t>Financial Statements</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>Purchases of Investments</t>
+        </is>
+      </c>
+      <c r="B123" t="n">
+        <v>-104151034.81954</v>
+      </c>
+      <c r="C123" t="n">
+        <v>-11997654000</v>
+      </c>
+      <c r="D123" t="n">
+        <v>0</v>
+      </c>
+      <c r="E123" t="n">
+        <v>81823000</v>
+      </c>
+      <c r="F123" t="n">
+        <v>346711949.2977287</v>
+      </c>
+      <c r="G123" t="inlineStr">
+        <is>
+          <t>Financial Statements</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>Research and Development Expenses</t>
+        </is>
+      </c>
+      <c r="B124" t="n">
+        <v>28169938.85242331</v>
+      </c>
+      <c r="C124" t="n">
+        <v>-214000</v>
+      </c>
+      <c r="D124" t="n">
+        <v>0</v>
+      </c>
+      <c r="E124" t="n">
+        <v>893000000</v>
+      </c>
+      <c r="F124" t="n">
+        <v>94071513.75079077</v>
+      </c>
+      <c r="G124" t="inlineStr">
+        <is>
+          <t>Financial Statements</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>Retained Earnings</t>
+        </is>
+      </c>
+      <c r="B125" t="n">
+        <v>3628393969.724315</v>
+      </c>
+      <c r="C125" t="n">
+        <v>-4839000000</v>
+      </c>
+      <c r="D125" t="n">
+        <v>1293100000</v>
+      </c>
+      <c r="E125" t="n">
+        <v>37899000000</v>
+      </c>
+      <c r="F125" t="n">
+        <v>6424744717.887364</v>
+      </c>
+      <c r="G125" t="inlineStr">
+        <is>
+          <t>Financial Statements</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>Revenue</t>
+        </is>
+      </c>
+      <c r="B126" t="n">
+        <v>2728749857.762843</v>
+      </c>
+      <c r="C126" t="n">
+        <v>-4273000</v>
+      </c>
+      <c r="D126" t="n">
+        <v>1297700000</v>
+      </c>
+      <c r="E126" t="n">
+        <v>25420000000</v>
+      </c>
+      <c r="F126" t="n">
+        <v>3959362594.26175</v>
+      </c>
+      <c r="G126" t="inlineStr">
+        <is>
+          <t>Financial Statements</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>Sales and Maturities of Investments</t>
+        </is>
+      </c>
+      <c r="B127" t="n">
+        <v>99796411.86111638</v>
+      </c>
+      <c r="C127" t="n">
+        <v>-9409000</v>
+      </c>
+      <c r="D127" t="n">
+        <v>0</v>
+      </c>
+      <c r="E127" t="n">
+        <v>8936406000</v>
+      </c>
+      <c r="F127" t="n">
+        <v>311292561.8781183</v>
+      </c>
+      <c r="G127" t="inlineStr">
+        <is>
+          <t>Financial Statements</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>Selling General and Administrative Expenses</t>
+        </is>
+      </c>
+      <c r="B128" t="n">
+        <v>296899614.9988182</v>
+      </c>
+      <c r="C128" t="n">
+        <v>-5054000</v>
+      </c>
+      <c r="D128" t="n">
+        <v>119600000</v>
+      </c>
+      <c r="E128" t="n">
+        <v>3343000000</v>
+      </c>
+      <c r="F128" t="n">
+        <v>486131457.7292245</v>
+      </c>
+      <c r="G128" t="inlineStr">
+        <is>
+          <t>Financial Statements</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>Selling and Marketing Expenses</t>
+        </is>
+      </c>
+      <c r="B129" t="n">
+        <v>25431647.83100381</v>
+      </c>
+      <c r="C129" t="n">
+        <v>-3003000</v>
+      </c>
+      <c r="D129" t="n">
+        <v>0</v>
+      </c>
+      <c r="E129" t="n">
+        <v>876761000</v>
+      </c>
+      <c r="F129" t="n">
+        <v>97367023.07782876</v>
+      </c>
+      <c r="G129" t="inlineStr">
+        <is>
+          <t>Financial Statements</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>Short Term Investments</t>
+        </is>
+      </c>
+      <c r="B130" t="n">
+        <v>182988242.5453949</v>
+      </c>
+      <c r="C130" t="n">
+        <v>-515000</v>
+      </c>
+      <c r="D130" t="n">
+        <v>0</v>
+      </c>
+      <c r="E130" t="n">
+        <v>6178000000</v>
+      </c>
+      <c r="F130" t="n">
+        <v>599747024.6501396</v>
+      </c>
+      <c r="G130" t="inlineStr">
+        <is>
+          <t>Financial Statements</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>Short-Term Debt</t>
+        </is>
+      </c>
+      <c r="B131" t="n">
+        <v>465870869.0188637</v>
+      </c>
+      <c r="C131" t="n">
+        <v>-655561</v>
+      </c>
+      <c r="D131" t="n">
+        <v>83800000</v>
+      </c>
+      <c r="E131" t="n">
+        <v>5363000000</v>
+      </c>
+      <c r="F131" t="n">
+        <v>885210679.511958</v>
+      </c>
+      <c r="G131" t="inlineStr">
+        <is>
+          <t>Financial Statements</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>Stock-Based Compensation</t>
+        </is>
+      </c>
+      <c r="B132" t="n">
+        <v>14496292.55192952</v>
+      </c>
+      <c r="C132" t="n">
+        <v>-36000000</v>
+      </c>
+      <c r="D132" t="n">
+        <v>5106000</v>
+      </c>
+      <c r="E132" t="n">
+        <v>254000000</v>
+      </c>
+      <c r="F132" t="n">
+        <v>29968462.79206444</v>
+      </c>
+      <c r="G132" t="inlineStr">
+        <is>
+          <t>Financial Statements</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>Tax Assets</t>
+        </is>
+      </c>
+      <c r="B133" t="n">
+        <v>378132518.5754565</v>
+      </c>
+      <c r="C133" t="n">
+        <v>-2310712000</v>
+      </c>
+      <c r="D133" t="n">
+        <v>48963000</v>
+      </c>
+      <c r="E133" t="n">
+        <v>6535000000</v>
+      </c>
+      <c r="F133" t="n">
+        <v>909237680.3453447</v>
+      </c>
+      <c r="G133" t="inlineStr">
+        <is>
+          <t>Financial Statements</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>Tax Payable</t>
+        </is>
+      </c>
+      <c r="B134" t="n">
+        <v>60670669.07187485</v>
+      </c>
+      <c r="C134" t="n">
+        <v>-87400</v>
+      </c>
+      <c r="D134" t="n">
+        <v>2810000</v>
+      </c>
+      <c r="E134" t="n">
+        <v>1187000000</v>
+      </c>
+      <c r="F134" t="n">
+        <v>150628980.4038844</v>
+      </c>
+      <c r="G134" t="inlineStr">
+        <is>
+          <t>Financial Statements</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>Total Assets</t>
+        </is>
+      </c>
+      <c r="B135" t="n">
+        <v>15592495985.54643</v>
+      </c>
+      <c r="C135" t="n">
+        <v>123279</v>
+      </c>
+      <c r="D135" t="n">
+        <v>7048475000</v>
+      </c>
+      <c r="E135" t="n">
+        <v>131119000000</v>
+      </c>
+      <c r="F135" t="n">
+        <v>21911032910.63581</v>
+      </c>
+      <c r="G135" t="inlineStr">
+        <is>
+          <t>Financial Statements</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>Total Current Assets</t>
+        </is>
+      </c>
+      <c r="B136" t="n">
+        <v>3937085272.106926</v>
+      </c>
+      <c r="C136" t="n">
+        <v>29954</v>
+      </c>
+      <c r="D136" t="n">
+        <v>1933750000</v>
+      </c>
+      <c r="E136" t="n">
+        <v>41276000000</v>
+      </c>
+      <c r="F136" t="n">
+        <v>5729273613.685635</v>
+      </c>
+      <c r="G136" t="inlineStr">
+        <is>
+          <t>Financial Statements</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>Total Current Liabilities</t>
+        </is>
+      </c>
+      <c r="B137" t="n">
+        <v>2811976684.335652</v>
+      </c>
+      <c r="C137" t="n">
+        <v>24083</v>
+      </c>
+      <c r="D137" t="n">
+        <v>1138200000</v>
+      </c>
+      <c r="E137" t="n">
+        <v>29919000000</v>
+      </c>
+      <c r="F137" t="n">
+        <v>4247045840.386281</v>
+      </c>
+      <c r="G137" t="inlineStr">
+        <is>
+          <t>Financial Statements</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>Total Debt</t>
+        </is>
+      </c>
+      <c r="B138" t="n">
+        <v>4593265532.65535</v>
+      </c>
+      <c r="C138" t="n">
+        <v>0</v>
+      </c>
+      <c r="D138" t="n">
+        <v>2019244000</v>
+      </c>
+      <c r="E138" t="n">
+        <v>37124000000</v>
+      </c>
+      <c r="F138" t="n">
+        <v>6254194800.162066</v>
+      </c>
+      <c r="G138" t="inlineStr">
+        <is>
+          <t>Financial Statements</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>Total Equity</t>
+        </is>
+      </c>
+      <c r="B139" t="n">
+        <v>4968502543.28632</v>
+      </c>
+      <c r="C139" t="n">
+        <v>-501467000</v>
+      </c>
+      <c r="D139" t="n">
+        <v>2095000000</v>
+      </c>
+      <c r="E139" t="n">
+        <v>49975000000</v>
+      </c>
+      <c r="F139" t="n">
+        <v>7272421518.553947</v>
+      </c>
+      <c r="G139" t="inlineStr">
+        <is>
+          <t>Financial Statements</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>Total Investments</t>
+        </is>
+      </c>
+      <c r="B140" t="n">
+        <v>729199594.637731</v>
+      </c>
+      <c r="C140" t="n">
+        <v>-334673000</v>
+      </c>
+      <c r="D140" t="n">
+        <v>43275000</v>
+      </c>
+      <c r="E140" t="n">
+        <v>19331000000</v>
+      </c>
+      <c r="F140" t="n">
+        <v>1944649108.256021</v>
+      </c>
+      <c r="G140" t="inlineStr">
+        <is>
+          <t>Financial Statements</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>Total Liabilities</t>
+        </is>
+      </c>
+      <c r="B141" t="n">
+        <v>9817545124.721975</v>
+      </c>
+      <c r="C141" t="n">
+        <v>79283</v>
+      </c>
+      <c r="D141" t="n">
+        <v>4308693000</v>
+      </c>
+      <c r="E141" t="n">
+        <v>87293000000</v>
+      </c>
+      <c r="F141" t="n">
+        <v>13527062565.41607</v>
+      </c>
+      <c r="G141" t="inlineStr">
+        <is>
+          <t>Financial Statements</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>Total Liabilities and Stockholders' Equity</t>
+        </is>
+      </c>
+      <c r="B142" t="n">
+        <v>15556696866.65008</v>
+      </c>
+      <c r="C142" t="n">
+        <v>123279</v>
+      </c>
+      <c r="D142" t="n">
+        <v>7043426000</v>
+      </c>
+      <c r="E142" t="n">
+        <v>131119000000</v>
+      </c>
+      <c r="F142" t="n">
+        <v>21905884302.05412</v>
+      </c>
+      <c r="G142" t="inlineStr">
+        <is>
+          <t>Financial Statements</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>Total Liabilities and Total Equity</t>
+        </is>
+      </c>
+      <c r="B143" t="n">
+        <v>15556696866.65008</v>
+      </c>
+      <c r="C143" t="n">
+        <v>123279</v>
+      </c>
+      <c r="D143" t="n">
+        <v>7043426000</v>
+      </c>
+      <c r="E143" t="n">
+        <v>131119000000</v>
+      </c>
+      <c r="F143" t="n">
+        <v>21905884302.05412</v>
+      </c>
+      <c r="G143" t="inlineStr">
+        <is>
+          <t>Financial Statements</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>Total Non-Current Assets</t>
+        </is>
+      </c>
+      <c r="B144" t="n">
+        <v>11011964229.48797</v>
+      </c>
+      <c r="C144" t="n">
+        <v>49861</v>
+      </c>
+      <c r="D144" t="n">
+        <v>4119200000</v>
+      </c>
+      <c r="E144" t="n">
+        <v>104263000000</v>
+      </c>
+      <c r="F144" t="n">
+        <v>15994777583.24965</v>
+      </c>
+      <c r="G144" t="inlineStr">
+        <is>
+          <t>Financial Statements</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>Total Non-Current Liabilities</t>
+        </is>
+      </c>
+      <c r="B145" t="n">
+        <v>6639451321.627382</v>
+      </c>
+      <c r="C145" t="n">
+        <v>53696</v>
+      </c>
+      <c r="D145" t="n">
+        <v>2809300000</v>
+      </c>
+      <c r="E145" t="n">
+        <v>54300000000</v>
+      </c>
+      <c r="F145" t="n">
+        <v>9424654097.471582</v>
+      </c>
+      <c r="G145" t="inlineStr">
+        <is>
+          <t>Financial Statements</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>Total Other Income Expenses Net</t>
+        </is>
+      </c>
+      <c r="B146" t="n">
+        <v>-13134652.92164943</v>
+      </c>
+      <c r="C146" t="n">
+        <v>-503976000</v>
+      </c>
+      <c r="D146" t="n">
+        <v>-920000</v>
+      </c>
+      <c r="E146" t="n">
+        <v>286000000</v>
+      </c>
+      <c r="F146" t="n">
+        <v>72414124.06600553</v>
+      </c>
+      <c r="G146" t="inlineStr">
+        <is>
+          <t>Financial Statements</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>Total Stockholders' Equity</t>
+        </is>
+      </c>
+      <c r="B147" t="n">
+        <v>4933321106.998609</v>
+      </c>
+      <c r="C147" t="n">
+        <v>-526491000</v>
+      </c>
+      <c r="D147" t="n">
+        <v>2088608000</v>
+      </c>
+      <c r="E147" t="n">
+        <v>49269000000</v>
+      </c>
+      <c r="F147" t="n">
+        <v>7194176771.14937</v>
+      </c>
+      <c r="G147" t="inlineStr">
+        <is>
+          <t>Financial Statements</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>Weighted Average Shares Outstanding</t>
+        </is>
+      </c>
+      <c r="B148" t="n">
+        <v>352790171.1679071</v>
+      </c>
+      <c r="C148" t="n">
+        <v>0</v>
+      </c>
+      <c r="D148" t="n">
+        <v>146000000</v>
+      </c>
+      <c r="E148" t="n">
+        <v>13751391147</v>
+      </c>
+      <c r="F148" t="n">
+        <v>720460888.9889255</v>
+      </c>
+      <c r="G148" t="inlineStr">
+        <is>
+          <t>Financial Statements</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>Weighted Average Shares Outstanding (Diluted)</t>
+        </is>
+      </c>
+      <c r="B149" t="n">
+        <v>316630108.9351969</v>
+      </c>
+      <c r="C149" t="n">
+        <v>0</v>
+      </c>
+      <c r="D149" t="n">
+        <v>145951913</v>
+      </c>
+      <c r="E149" t="n">
+        <v>13986214405</v>
+      </c>
+      <c r="F149" t="n">
+        <v>547337219.461812</v>
+      </c>
+      <c r="G149" t="inlineStr">
+        <is>
+          <t>Financial Statements</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>Market Capitalization</t>
+        </is>
+      </c>
+      <c r="B150" t="n">
+        <v>18996749034.57488</v>
+      </c>
+      <c r="C150" t="n">
+        <v>106422</v>
+      </c>
+      <c r="D150" t="n">
+        <v>6409459125</v>
+      </c>
+      <c r="E150" t="n">
+        <v>726320349360</v>
+      </c>
+      <c r="F150" t="n">
+        <v>44246873159.19034</v>
+      </c>
+      <c r="G150" t="inlineStr">
+        <is>
+          <t>Market Capitalization</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>Days Since Call</t>
+        </is>
+      </c>
+      <c r="B151" t="n">
+        <v>58.38936286077328</v>
+      </c>
+      <c r="C151" t="n">
+        <v>0</v>
+      </c>
+      <c r="D151" t="n">
+        <v>61</v>
+      </c>
+      <c r="E151" t="n">
+        <v>91</v>
+      </c>
+      <c r="F151" t="n">
+        <v>13.04928800095301</v>
+      </c>
+      <c r="G151" t="inlineStr">
+        <is>
+          <t>Metadata</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>FinBERT Positivity Score</t>
+        </is>
+      </c>
+      <c r="B152" t="n">
+        <v>0.5330976029111905</v>
+      </c>
+      <c r="C152" t="n">
+        <v>-0.2811957506790093</v>
+      </c>
+      <c r="D152" t="n">
+        <v>0.5244551335152926</v>
+      </c>
+      <c r="E152" t="n">
+        <v>1.612783856719735</v>
+      </c>
+      <c r="F152" t="n">
+        <v>0.2541366314098529</v>
+      </c>
+      <c r="G152" t="inlineStr">
+        <is>
+          <t>NLP Feature</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>First Principal Component of Tone</t>
+        </is>
+      </c>
+      <c r="B153" t="n">
+        <v>-0.03433016859819993</v>
+      </c>
+      <c r="C153" t="n">
+        <v>-2.912620748125866</v>
+      </c>
+      <c r="D153" t="n">
+        <v>-0.2222630379774446</v>
+      </c>
+      <c r="E153" t="n">
+        <v>10.33449805186935</v>
+      </c>
+      <c r="F153" t="n">
+        <v>1.284823876635564</v>
+      </c>
+      <c r="G153" t="inlineStr">
+        <is>
+          <t>NLP Feature</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>Gunning-Fog Score</t>
+        </is>
+      </c>
+      <c r="B154" t="n">
+        <v>12.5037332829149</v>
+      </c>
+      <c r="C154" t="n">
+        <v>8.551054692434002</v>
+      </c>
+      <c r="D154" t="n">
+        <v>12.41398083122072</v>
+      </c>
+      <c r="E154" t="n">
+        <v>19.28576584705617</v>
+      </c>
+      <c r="F154" t="n">
+        <v>1.313901380517324</v>
+      </c>
+      <c r="G154" t="inlineStr">
+        <is>
+          <t>NLP Feature</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>Number of Questions</t>
+        </is>
+      </c>
+      <c r="B155" t="n">
+        <v>36.50299509892903</v>
+      </c>
+      <c r="C155" t="n">
+        <v>0</v>
+      </c>
+      <c r="D155" t="n">
+        <v>35</v>
+      </c>
+      <c r="E155" t="n">
+        <v>107</v>
+      </c>
+      <c r="F155" t="n">
+        <v>16.38001421719229</v>
+      </c>
+      <c r="G155" t="inlineStr">
+        <is>
+          <t>NLP Feature</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>Number of Questions Divided By Call Word Count</t>
+        </is>
+      </c>
+      <c r="B156" t="n">
+        <v>0.004131912107721218</v>
+      </c>
+      <c r="C156" t="n">
+        <v>0</v>
+      </c>
+      <c r="D156" t="n">
+        <v>0.003999304468788037</v>
+      </c>
+      <c r="E156" t="n">
+        <v>0.01297152229014462</v>
+      </c>
+      <c r="F156" t="n">
+        <v>0.001505049118045665</v>
+      </c>
+      <c r="G156" t="inlineStr">
+        <is>
+          <t>NLP Feature</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>Numeric Transparency</t>
+        </is>
+      </c>
+      <c r="B157" t="n">
+        <v>0.1224305681611908</v>
+      </c>
+      <c r="C157" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D157" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="E157" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="F157" t="n">
+        <v>0.04643060957498905</v>
+      </c>
+      <c r="G157" t="inlineStr">
+        <is>
+          <t>NLP Feature</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>Word Count</t>
+        </is>
+      </c>
+      <c r="B158" t="n">
+        <v>8834.147576692685</v>
+      </c>
+      <c r="C158" t="n">
+        <v>525</v>
+      </c>
+      <c r="D158" t="n">
+        <v>9083</v>
+      </c>
+      <c r="E158" t="n">
+        <v>22006</v>
+      </c>
+      <c r="F158" t="n">
+        <v>2471.868714867427</v>
+      </c>
+      <c r="G158" t="inlineStr">
+        <is>
+          <t>NLP Feature</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
           <t>Change Since Last Fixed Quarter Date</t>
         </is>
       </c>
-      <c r="B113" t="n">
-        <v>0.007760141093474427</v>
-      </c>
-      <c r="C113" t="n">
+      <c r="B159" t="n">
+        <v>0.00925757850789617</v>
+      </c>
+      <c r="C159" t="n">
         <v>-2</v>
       </c>
-      <c r="D113" t="n">
+      <c r="D159" t="n">
         <v>0</v>
       </c>
-      <c r="E113" t="n">
+      <c r="E159" t="n">
         <v>2</v>
       </c>
-      <c r="F113" t="n">
-        <v>0.2661799147355614</v>
-      </c>
-      <c r="G113" t="inlineStr">
+      <c r="F159" t="n">
+        <v>0.2635327364417582</v>
+      </c>
+      <c r="G159" t="inlineStr">
         <is>
           <t>Predicted - Change</t>
         </is>

</xml_diff>